<commit_message>
update doc with more explicit + normalization/left factorization combination
</commit_message>
<xml_diff>
--- a/doc/ops.xlsx
+++ b/doc/ops.xlsx
@@ -12,7 +12,7 @@
     <sheet name="stack op 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'stack op'!$A$27:$M$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'stack op'!$A$31:$M$59</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'stack op 2'!$A$27:$M$66</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="179">
   <si>
     <t>A → α β+ γ</t>
   </si>
@@ -938,6 +938,53 @@
       </rPr>
       <t xml:space="preserve"> R: collects [α]</t>
     </r>
+  </si>
+  <si>
+    <t>A → α β* γ δ* ζ</t>
+  </si>
+  <si>
+    <t>child_+*(A)</t>
+  </si>
+  <si>
+    <t>child_fact(A1)</t>
+  </si>
+  <si>
+    <t>child_+*(A)
+|child_fact(A1)</t>
+  </si>
+  <si>
+    <t>child_+*(A)
+parent_fact</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L: exit_A2 → iter_A(ctx={β}) </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R: collects all βs into an array</t>
+    </r>
+  </si>
+  <si>
+    <t>(&amp; left factorization)</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1443,11 +1490,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1803,92 +1883,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2193,22 +2308,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="19" customWidth="1"/>
     <col min="7" max="11" width="7.5703125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="87.140625" style="57" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.5703125" style="4" customWidth="1"/>
     <col min="15" max="20" width="9.140625" style="4"/>
@@ -2221,14 +2336,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="148" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -2293,8 +2408,8 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="130" t="s">
-        <v>102</v>
+      <c r="L3" s="138" t="s">
+        <v>173</v>
       </c>
       <c r="M3" s="57" t="s">
         <v>117</v>
@@ -2302,7 +2417,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="143"/>
-      <c r="D4" s="144"/>
+      <c r="D4" s="143"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -2313,229 +2428,210 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="131"/>
+      <c r="L4" s="138"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="143"/>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="145" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="166" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="143"/>
+      <c r="E5" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="168" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="168" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="59" t="s">
+      <c r="J5" s="168"/>
+      <c r="K5" s="168"/>
+      <c r="L5" s="169"/>
+      <c r="M5" s="170" t="s">
         <v>118</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N5" s="171"/>
+      <c r="O5" s="171"/>
+      <c r="P5" s="171"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="171"/>
+      <c r="S5" s="171"/>
+      <c r="T5" s="171"/>
+    </row>
+    <row r="6" spans="1:20" s="160" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="143"/>
       <c r="D6" s="143"/>
-      <c r="E6" t="s">
+      <c r="E6" s="161" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="165" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+      <c r="L6" s="130" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6" s="163"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="143"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="138" t="s">
+        <v>174</v>
+      </c>
+      <c r="M7" s="57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="143"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="151"/>
+    </row>
+    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="143"/>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="147" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="M6" s="57" t="s">
+      <c r="L10" s="138" t="s">
+        <v>173</v>
+      </c>
+      <c r="M10" s="57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="146"/>
-      <c r="D7" s="146"/>
-      <c r="E7" t="s">
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="131"/>
-    </row>
-    <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="143"/>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="145" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="146"/>
-      <c r="D11" s="146"/>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="57" t="s">
-        <v>112</v>
-      </c>
+      <c r="L11" s="151"/>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="48"/>
+        <v>14</v>
+      </c>
+      <c r="D12" s="142" t="s">
+        <v>81</v>
+      </c>
       <c r="E12" s="25" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="117"/>
+        <v>18</v>
+      </c>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="119"/>
       <c r="M12" s="60" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
@@ -2547,808 +2643,826 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="143"/>
-      <c r="D13" s="50"/>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="143"/>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="143"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="147" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="116"/>
-      <c r="M13" s="57" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="122"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-    </row>
-    <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="7" t="s">
+      <c r="H14" s="44"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="46"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="142" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="7" t="s">
+      <c r="C16" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="44" t="s">
+      <c r="H16" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" t="s">
-        <v>137</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="116"/>
-      <c r="M16" s="62" t="s">
-        <v>111</v>
-      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="143"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="116"/>
+      <c r="M17" s="57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="143"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F18" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="116"/>
-      <c r="M17" s="62"/>
-    </row>
-    <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="7" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+    </row>
+    <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="143"/>
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="C19" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="118"/>
-      <c r="M18" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="116"/>
-      <c r="M19" s="62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="146"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="143"/>
       <c r="B20" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="116"/>
+      <c r="M20" s="62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="143"/>
+      <c r="D21" s="50"/>
+      <c r="E21" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="116"/>
-    </row>
-    <row r="21" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="142" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="33" t="s">
+      <c r="L21" s="116"/>
+      <c r="M21" s="62"/>
+    </row>
+    <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="143"/>
+      <c r="B22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="51"/>
+      <c r="E22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="117"/>
-      <c r="M21" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="D22" s="50"/>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="116"/>
-      <c r="M22" s="64" t="s">
-        <v>107</v>
-      </c>
+      <c r="H22" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="143"/>
+      <c r="B23" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D23" s="50"/>
       <c r="E23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>63</v>
+      <c r="H23" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="46" t="s">
+        <v>18</v>
       </c>
       <c r="L23" s="116"/>
-      <c r="M23" s="57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
+      <c r="M23" s="62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="144"/>
+      <c r="B24" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D24" s="50"/>
       <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="116"/>
+    </row>
+    <row r="25" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="142" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="143"/>
+      <c r="D26" s="50"/>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="116"/>
+      <c r="M26" s="64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="143"/>
+      <c r="D27" s="50"/>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L27" s="116"/>
+      <c r="M27" s="57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="143"/>
+      <c r="D28" s="50"/>
+      <c r="E28" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F28" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="116"/>
-      <c r="M24" s="57" t="s">
+      <c r="L28" s="116"/>
+      <c r="M28" s="57" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="146"/>
-      <c r="D25" s="50"/>
-      <c r="E25" t="s">
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="144"/>
+      <c r="D29" s="50"/>
+      <c r="E29" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="123"/>
-      <c r="M25" s="57" t="s">
+      <c r="L29" s="123"/>
+      <c r="M29" s="57" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="86" t="s">
+    <row r="30" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-    </row>
-    <row r="27" spans="1:20" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+    </row>
+    <row r="31" spans="1:20" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="75" t="s">
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="M27" s="75" t="s">
+      <c r="M31" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="N27" s="76"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="76"/>
-    </row>
-    <row r="28" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="N31" s="76"/>
+      <c r="O31" s="76"/>
+      <c r="P31" s="76"/>
+      <c r="Q31" s="76"/>
+      <c r="R31" s="76"/>
+      <c r="S31" s="76"/>
+      <c r="T31" s="76"/>
+    </row>
+    <row r="32" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="74" t="s">
+      <c r="C32" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E32" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F32" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G32" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="77" t="s">
+      <c r="H32" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="77" t="s">
+      <c r="J32" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K32" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="L28" s="117"/>
-      <c r="M28" s="60" t="s">
+      <c r="L32" s="117"/>
+      <c r="M32" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="132" t="s">
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D33" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E33" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F33" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="67" t="s">
+      <c r="G33" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H33" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="M29" s="57" t="s">
+      <c r="L33" s="138" t="s">
+        <v>173</v>
+      </c>
+      <c r="M33" s="57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="133"/>
-      <c r="E30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="66" t="s">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D34" s="146"/>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="130"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="132" t="s">
+      <c r="L34" s="138"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D35" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E35" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="66" t="s">
+      <c r="F35" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="67" t="s">
+      <c r="G35" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H35" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="130"/>
-      <c r="M31" s="57" t="s">
+      <c r="L35" s="138"/>
+      <c r="M35" s="57" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="133"/>
-      <c r="E32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="66" t="s">
+    <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="146"/>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="L32" s="134"/>
-    </row>
-    <row r="33" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
+      <c r="L36" s="139"/>
+    </row>
+    <row r="37" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C37" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E37" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="150" t="s">
+      <c r="F37" s="131" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="151" t="s">
+      <c r="G37" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="152" t="s">
+      <c r="H37" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="117" t="s">
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="M33" s="60" t="s">
+      <c r="M37" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="132" t="s">
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D38" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E38" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="66" t="s">
+      <c r="F38" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G38" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="46" t="s">
+      <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="130" t="s">
-        <v>131</v>
-      </c>
-      <c r="M34" s="57" t="s">
+      <c r="L38" s="138" t="s">
+        <v>173</v>
+      </c>
+      <c r="M38" s="57" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="133"/>
-      <c r="E35" t="s">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D39" s="146"/>
+      <c r="E39" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="66" t="s">
+      <c r="F39" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="65"/>
-      <c r="L35" s="130"/>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D36" s="132" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="L36" s="130" t="s">
-        <v>103</v>
-      </c>
-      <c r="M36" s="57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="133"/>
-      <c r="E37" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="83" t="s">
-        <v>69</v>
-      </c>
-      <c r="L37" s="134"/>
-    </row>
-    <row r="38" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="117" t="s">
-        <v>161</v>
-      </c>
-      <c r="M38" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="31"/>
-      <c r="Q38" s="31"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="31"/>
-      <c r="T38" s="31"/>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="92" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" t="s">
-        <v>125</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="L39" s="125" t="s">
-        <v>160</v>
-      </c>
-      <c r="M39" s="57" t="s">
-        <v>156</v>
-      </c>
+      <c r="H39" s="65"/>
+      <c r="L39" s="138"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="132" t="s">
+      <c r="D40" s="145" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="130" t="s">
+      <c r="L40" s="138" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D41" s="133"/>
+    <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="146"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="130"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D42" s="132" t="s">
+      <c r="L41" s="139"/>
+    </row>
+    <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="117" t="s">
+        <v>161</v>
+      </c>
+      <c r="M42" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
+      <c r="T42" s="31"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D43" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43" s="125" t="s">
+        <v>160</v>
+      </c>
+      <c r="M43" s="57" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D44" s="145" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L44" s="138" t="s">
+        <v>103</v>
+      </c>
+      <c r="M44" s="57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D45" s="146"/>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L45" s="138"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D46" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E46" t="s">
         <v>126</v>
-      </c>
-      <c r="F42" s="95" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="93" t="s">
-        <v>170</v>
-      </c>
-      <c r="L42" s="136" t="s">
-        <v>158</v>
-      </c>
-      <c r="M42" s="57" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="137"/>
-      <c r="E43" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" s="103" t="s">
-        <v>170</v>
-      </c>
-      <c r="L43" s="134"/>
-      <c r="M43" s="57" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I44" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="117" t="s">
-        <v>161</v>
-      </c>
-      <c r="M44" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="31"/>
-      <c r="T44" s="31"/>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="92" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" s="98" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="125" t="s">
-        <v>160</v>
-      </c>
-      <c r="M45" s="57" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D46" s="132" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>139</v>
       </c>
       <c r="F46" s="95" t="s">
         <v>79</v>
       </c>
       <c r="G46" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="L46" s="136" t="s">
-        <v>158</v>
+        <v>170</v>
+      </c>
+      <c r="L46" s="152" t="s">
+        <v>175</v>
       </c>
       <c r="M46" s="57" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="133"/>
-      <c r="E47" s="42" t="s">
-        <v>91</v>
+      <c r="D47" s="153"/>
+      <c r="E47" t="s">
+        <v>127</v>
       </c>
       <c r="F47" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="L47" s="134"/>
+        <v>170</v>
+      </c>
+      <c r="L47" s="139"/>
       <c r="M47" s="57" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48" s="154" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E48" s="74" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F48" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="152" t="s">
+      <c r="I48" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
       <c r="J48" s="27"/>
       <c r="K48" s="27"/>
-      <c r="L48" s="153" t="s">
-        <v>160</v>
+      <c r="L48" s="117" t="s">
+        <v>161</v>
       </c>
       <c r="M48" s="60" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="N48" s="31"/>
       <c r="O48" s="31"/>
@@ -3359,60 +3473,56 @@
       <c r="T48" s="31"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D49" s="92" t="s">
+        <v>17</v>
+      </c>
       <c r="E49" s="42" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="L49" s="116"/>
+        <v>47</v>
+      </c>
+      <c r="G49" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="125" t="s">
+        <v>160</v>
+      </c>
       <c r="M49" s="57" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="132" t="s">
+      <c r="D50" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="E50" t="s">
-        <v>149</v>
+      <c r="E50" s="42" t="s">
+        <v>139</v>
       </c>
       <c r="F50" s="95" t="s">
-        <v>80</v>
-      </c>
-      <c r="G50" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="H50" s="105" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" s="130" t="s">
-        <v>162</v>
+      <c r="L50" s="152" t="s">
+        <v>175</v>
       </c>
       <c r="M50" s="57" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="133"/>
-      <c r="E51" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G51" s="111" t="s">
+      <c r="D51" s="146"/>
+      <c r="E51" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F51" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="H51" s="115" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="134"/>
+      <c r="L51" s="139"/>
       <c r="M51" s="57" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -3420,31 +3530,29 @@
         <v>145</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="154" t="s">
+        <v>140</v>
+      </c>
+      <c r="D52" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="25" t="s">
-        <v>15</v>
+      <c r="E52" s="74" t="s">
+        <v>40</v>
       </c>
       <c r="F52" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G52" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="133" t="s">
         <v>18</v>
       </c>
+      <c r="H52" s="27"/>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
-      <c r="L52" s="117" t="s">
-        <v>81</v>
+      <c r="L52" s="134" t="s">
+        <v>160</v>
       </c>
       <c r="M52" s="60" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="N52" s="31"/>
       <c r="O52" s="31"/>
@@ -3456,66 +3564,92 @@
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E53" s="42" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L53" s="116"/>
+      <c r="M53" s="57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D54" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>149</v>
+      </c>
+      <c r="F54" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="G54" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L53" s="116" t="s">
-        <v>160</v>
-      </c>
-      <c r="M53" s="57" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="155" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" s="95" t="s">
+      <c r="L54" s="138" t="s">
+        <v>162</v>
+      </c>
+      <c r="M54" s="57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="146"/>
+      <c r="E55" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="G55" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="105" t="s">
+      <c r="H55" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L54" s="130" t="s">
-        <v>167</v>
-      </c>
-      <c r="M54" s="57" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="156"/>
-      <c r="E55" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="F55" s="157" t="s">
-        <v>29</v>
-      </c>
-      <c r="G55" s="158" t="s">
-        <v>64</v>
-      </c>
-      <c r="L55" s="134"/>
+      <c r="L55" s="139"/>
       <c r="M55" s="57" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F56" s="26"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
+      <c r="B56" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" s="135" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="27" t="s">
+        <v>18</v>
+      </c>
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="60"/>
+      <c r="L56" s="117" t="s">
+        <v>81</v>
+      </c>
+      <c r="M56" s="60" t="s">
+        <v>85</v>
+      </c>
       <c r="N56" s="31"/>
       <c r="O56" s="31"/>
       <c r="P56" s="31"/>
@@ -3524,36 +3658,107 @@
       <c r="S56" s="31"/>
       <c r="T56" s="31"/>
     </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E57" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" s="116" t="s">
+        <v>160</v>
+      </c>
+      <c r="M57" s="57" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D58" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" s="95" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" s="138" t="s">
+        <v>167</v>
+      </c>
+      <c r="M58" s="57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="141"/>
+      <c r="E59" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F59" s="136" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="137" t="s">
+        <v>64</v>
+      </c>
+      <c r="L59" s="139"/>
+      <c r="M59" s="57" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="26"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="60"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
+      <c r="P60" s="31"/>
+      <c r="Q60" s="31"/>
+      <c r="R60" s="31"/>
+      <c r="S60" s="31"/>
+      <c r="T60" s="31"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="L54:L55"/>
+  <mergeCells count="29">
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="D50:D51"/>
     <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="L33:L36"/>
+    <mergeCell ref="L38:L39"/>
     <mergeCell ref="L40:L41"/>
-    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="L44:L45"/>
     <mergeCell ref="L46:L47"/>
     <mergeCell ref="L50:L51"/>
-    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D44:D45"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3589,20 +3794,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="147" t="s">
+      <c r="F1" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="149"/>
-      <c r="N1" s="147" t="s">
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="156"/>
+      <c r="N1" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="148"/>
-      <c r="P1" s="148"/>
-      <c r="Q1" s="148"/>
-      <c r="R1" s="149"/>
+      <c r="O1" s="155"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="155"/>
+      <c r="R1" s="156"/>
     </row>
     <row r="2" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
@@ -3782,7 +3987,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="146"/>
+      <c r="A7" s="144"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -3838,7 +4043,7 @@
       <c r="AA8" s="31"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="146"/>
+      <c r="A9" s="144"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -4096,7 +4301,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="146"/>
+      <c r="A19" s="144"/>
       <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
@@ -4259,7 +4464,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="146"/>
+      <c r="A27" s="144"/>
       <c r="D27" t="s">
         <v>49</v>
       </c>
@@ -4396,14 +4601,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="148" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -4468,7 +4673,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="130" t="s">
+      <c r="L3" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -4477,7 +4682,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="143"/>
-      <c r="D4" s="144"/>
+      <c r="D4" s="150"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -4488,7 +4693,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="131"/>
+      <c r="L4" s="151"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
@@ -4501,7 +4706,7 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="145" t="s">
+      <c r="D5" s="147" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4548,7 +4753,7 @@
       <c r="H6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="130" t="s">
+      <c r="L6" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="57" t="s">
@@ -4556,15 +4761,15 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="146"/>
-      <c r="D7" s="146"/>
+      <c r="A7" s="144"/>
+      <c r="D7" s="144"/>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="131"/>
+      <c r="L7" s="151"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="142" t="s">
@@ -4633,7 +4838,7 @@
       <c r="A10" s="143"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
-      <c r="D10" s="145" t="s">
+      <c r="D10" s="147" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -4662,8 +4867,8 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="146"/>
-      <c r="D11" s="146"/>
+      <c r="A11" s="144"/>
+      <c r="D11" s="144"/>
       <c r="E11" t="s">
         <v>16</v>
       </c>
@@ -4904,7 +5109,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="146"/>
+      <c r="A20" s="144"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -5005,7 +5210,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="146"/>
+      <c r="A25" s="144"/>
       <c r="D25" s="50"/>
       <c r="E25" t="s">
         <v>49</v>
@@ -5105,7 +5310,7 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="132" t="s">
+      <c r="D29" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
@@ -5120,7 +5325,7 @@
       <c r="H29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="130" t="s">
+      <c r="L29" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M29" s="57" t="s">
@@ -5128,7 +5333,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="133"/>
+      <c r="D30" s="146"/>
       <c r="E30" t="s">
         <v>4</v>
       </c>
@@ -5138,10 +5343,10 @@
       <c r="G30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="130"/>
+      <c r="L30" s="138"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="132" t="s">
+      <c r="D31" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
@@ -5156,13 +5361,13 @@
       <c r="H31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="130"/>
+      <c r="L31" s="138"/>
       <c r="M31" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="133"/>
+      <c r="D32" s="146"/>
       <c r="E32" t="s">
         <v>49</v>
       </c>
@@ -5172,7 +5377,7 @@
       <c r="G32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L32" s="134"/>
+      <c r="L32" s="139"/>
     </row>
     <row r="33" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
@@ -5230,7 +5435,7 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="132" t="s">
+      <c r="D35" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -5245,7 +5450,7 @@
       <c r="H35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="130" t="s">
+      <c r="L35" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="57" t="s">
@@ -5253,7 +5458,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="138"/>
+      <c r="D36" s="159"/>
       <c r="E36" s="43" t="s">
         <v>3</v>
       </c>
@@ -5262,7 +5467,7 @@
       </c>
       <c r="G36" s="46"/>
       <c r="H36" s="65"/>
-      <c r="L36" s="135"/>
+      <c r="L36" s="158"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D37" s="70" t="s">
@@ -5291,7 +5496,7 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="132" t="s">
+      <c r="D38" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -5306,7 +5511,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="130" t="s">
+      <c r="L38" s="138" t="s">
         <v>131</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -5314,7 +5519,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="133"/>
+      <c r="D39" s="146"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -5322,10 +5527,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="130"/>
+      <c r="L39" s="138"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="132" t="s">
+      <c r="D40" s="145" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -5343,7 +5548,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="130" t="s">
+      <c r="L40" s="138" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -5351,14 +5556,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="133"/>
+      <c r="D41" s="146"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="134"/>
+      <c r="L41" s="139"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -5400,7 +5605,7 @@
       <c r="T42" s="31"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="132" t="s">
+      <c r="D43" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
@@ -5415,7 +5620,7 @@
       <c r="H43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="130" t="s">
+      <c r="L43" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -5423,7 +5628,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="133"/>
+      <c r="D44" s="146"/>
       <c r="E44" t="s">
         <v>124</v>
       </c>
@@ -5433,13 +5638,13 @@
       <c r="G44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="130"/>
+      <c r="L44" s="138"/>
       <c r="M44" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="132" t="s">
+      <c r="D45" s="145" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -5457,7 +5662,7 @@
       <c r="I45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="130" t="s">
+      <c r="L45" s="138" t="s">
         <v>103</v>
       </c>
       <c r="M45" s="57" t="s">
@@ -5465,14 +5670,14 @@
       </c>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="138"/>
+      <c r="D46" s="159"/>
       <c r="E46" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L46" s="135"/>
+      <c r="L46" s="158"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D47" s="70" t="s">
@@ -5521,7 +5726,7 @@
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="132" t="s">
+      <c r="D49" s="145" t="s">
         <v>73</v>
       </c>
       <c r="E49" t="s">
@@ -5539,7 +5744,7 @@
       <c r="I49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="130" t="s">
+      <c r="L49" s="138" t="s">
         <v>103</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -5547,17 +5752,17 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="133"/>
+      <c r="D50" s="146"/>
       <c r="E50" t="s">
         <v>91</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="130"/>
+      <c r="L50" s="138"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D51" s="132" t="s">
+      <c r="D51" s="145" t="s">
         <v>74</v>
       </c>
       <c r="E51" t="s">
@@ -5569,7 +5774,7 @@
       <c r="G51" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L51" s="136" t="s">
+      <c r="L51" s="152" t="s">
         <v>158</v>
       </c>
       <c r="M51" s="57" t="s">
@@ -5577,14 +5782,14 @@
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="137"/>
+      <c r="D52" s="153"/>
       <c r="E52" t="s">
         <v>127</v>
       </c>
       <c r="F52" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="134"/>
+      <c r="L52" s="139"/>
       <c r="M52" s="57" t="s">
         <v>154</v>
       </c>
@@ -5631,7 +5836,7 @@
       <c r="T53" s="31"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="132" t="s">
+      <c r="D54" s="145" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="42" t="s">
@@ -5646,7 +5851,7 @@
       <c r="H54" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="130" t="s">
+      <c r="L54" s="138" t="s">
         <v>102</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -5654,7 +5859,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="139"/>
+      <c r="D55" s="157"/>
       <c r="E55" s="42" t="s">
         <v>4</v>
       </c>
@@ -5665,7 +5870,7 @@
         <v>19</v>
       </c>
       <c r="H55" s="46"/>
-      <c r="L55" s="135"/>
+      <c r="L55" s="158"/>
       <c r="M55" s="57" t="s">
         <v>152</v>
       </c>
@@ -5719,7 +5924,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="132" t="s">
+      <c r="D58" s="145" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -5731,7 +5936,7 @@
       <c r="G58" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="136" t="s">
+      <c r="L58" s="152" t="s">
         <v>158</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -5739,14 +5944,14 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="133"/>
+      <c r="D59" s="146"/>
       <c r="E59" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F59" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="134"/>
+      <c r="L59" s="139"/>
       <c r="M59" s="57" t="s">
         <v>152</v>
       </c>
@@ -5870,7 +6075,7 @@
       </c>
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D65" s="132" t="s">
+      <c r="D65" s="145" t="s">
         <v>74</v>
       </c>
       <c r="E65" t="s">
@@ -5885,7 +6090,7 @@
       <c r="H65" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L65" s="130" t="s">
+      <c r="L65" s="138" t="s">
         <v>162</v>
       </c>
       <c r="M65" s="57" t="s">
@@ -5893,7 +6098,7 @@
       </c>
     </row>
     <row r="66" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="133"/>
+      <c r="D66" s="146"/>
       <c r="E66" t="s">
         <v>150</v>
       </c>
@@ -5906,7 +6111,7 @@
       <c r="H66" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L66" s="134"/>
+      <c r="L66" s="139"/>
       <c r="M66" s="57" t="s">
         <v>147</v>
       </c>
@@ -5930,6 +6135,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="L45:L46"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D65:D66"/>
@@ -5940,30 +6169,6 @@
     <mergeCell ref="L51:L52"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L54:L55"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix parent and flag in cascaded left factorizations
</commit_message>
<xml_diff>
--- a/doc/ops.xlsx
+++ b/doc/ops.xlsx
@@ -1906,104 +1906,104 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2310,8 +2310,8 @@
   </sheetPr>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,14 +2336,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="148" t="s">
+      <c r="F1" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="157" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -2361,7 +2361,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="142" t="s">
+      <c r="D2" s="157" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -2394,8 +2394,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="143"/>
-      <c r="D3" s="143"/>
+      <c r="A3" s="158"/>
+      <c r="D3" s="158"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="138" t="s">
+      <c r="L3" s="150" t="s">
         <v>173</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -2416,8 +2416,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="143"/>
-      <c r="D4" s="143"/>
+      <c r="A4" s="158"/>
+      <c r="D4" s="158"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -2428,70 +2428,70 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="138"/>
+      <c r="L4" s="150"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="166" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143"/>
-      <c r="B5" s="166" t="s">
+    <row r="5" spans="1:20" s="144" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="158"/>
+      <c r="B5" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="143"/>
-      <c r="E5" s="166" t="s">
+      <c r="D5" s="158"/>
+      <c r="E5" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="167" t="s">
+      <c r="F5" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="168" t="s">
+      <c r="G5" s="146" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="168" t="s">
+      <c r="H5" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="168" t="s">
+      <c r="I5" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="168"/>
-      <c r="K5" s="168"/>
-      <c r="L5" s="169"/>
-      <c r="M5" s="170" t="s">
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="148" t="s">
         <v>118</v>
       </c>
-      <c r="N5" s="171"/>
-      <c r="O5" s="171"/>
-      <c r="P5" s="171"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="171"/>
-      <c r="S5" s="171"/>
-      <c r="T5" s="171"/>
-    </row>
-    <row r="6" spans="1:20" s="160" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="161" t="s">
+      <c r="N5" s="149"/>
+      <c r="O5" s="149"/>
+      <c r="P5" s="149"/>
+      <c r="Q5" s="149"/>
+      <c r="R5" s="149"/>
+      <c r="S5" s="149"/>
+      <c r="T5" s="149"/>
+    </row>
+    <row r="6" spans="1:20" s="138" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="164" t="s">
+      <c r="F6" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="165" t="s">
+      <c r="G6" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="162"/>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
       <c r="L6" s="130" t="s">
         <v>178</v>
       </c>
-      <c r="M6" s="163"/>
+      <c r="M6" s="141"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="D7" s="143"/>
+      <c r="A7" s="158"/>
+      <c r="D7" s="158"/>
       <c r="E7" s="42" t="s">
         <v>139</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="I7" s="46"/>
       <c r="J7" s="46"/>
       <c r="K7" s="46"/>
-      <c r="L7" s="138" t="s">
+      <c r="L7" s="150" t="s">
         <v>174</v>
       </c>
       <c r="M7" s="57" t="s">
@@ -2513,8 +2513,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="D8" s="150"/>
+      <c r="A8" s="158"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="42" t="s">
         <v>91</v>
       </c>
@@ -2529,14 +2529,14 @@
       <c r="L8" s="151"/>
     </row>
     <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="147" t="s">
+      <c r="D9" s="162" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -2569,8 +2569,8 @@
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
-      <c r="D10" s="143"/>
+      <c r="A10" s="158"/>
+      <c r="D10" s="158"/>
       <c r="E10" t="s">
         <v>2</v>
       </c>
@@ -2583,7 +2583,7 @@
       <c r="H10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="138" t="s">
+      <c r="L10" s="150" t="s">
         <v>173</v>
       </c>
       <c r="M10" s="57" t="s">
@@ -2591,8 +2591,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144"/>
-      <c r="D11" s="144"/>
+      <c r="A11" s="163"/>
+      <c r="D11" s="163"/>
       <c r="E11" t="s">
         <v>3</v>
       </c>
@@ -2602,7 +2602,7 @@
       <c r="L11" s="151"/>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="142" t="s">
+      <c r="A12" s="157" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -2611,7 +2611,7 @@
       <c r="C12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="142" t="s">
+      <c r="D12" s="157" t="s">
         <v>81</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -2642,11 +2642,11 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
+      <c r="A13" s="158"/>
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="143"/>
+      <c r="D13" s="158"/>
       <c r="E13" t="s">
         <v>16</v>
       </c>
@@ -2665,10 +2665,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="43"/>
       <c r="C14" s="43"/>
-      <c r="D14" s="147" t="s">
+      <c r="D14" s="162" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -2697,8 +2697,8 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="144"/>
-      <c r="D15" s="144"/>
+      <c r="A15" s="163"/>
+      <c r="D15" s="163"/>
       <c r="E15" t="s">
         <v>16</v>
       </c>
@@ -2718,7 +2718,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="157" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -2756,7 +2756,7 @@
       <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
+      <c r="A17" s="158"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>21</v>
@@ -2776,7 +2776,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
+      <c r="A18" s="158"/>
       <c r="D18" s="52"/>
       <c r="E18" s="53" t="s">
         <v>3</v>
@@ -2800,7 +2800,7 @@
       <c r="T18" s="56"/>
     </row>
     <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
+      <c r="A19" s="158"/>
       <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2836,7 +2836,7 @@
       <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
+      <c r="A20" s="158"/>
       <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
@@ -2862,7 +2862,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
+      <c r="A21" s="158"/>
       <c r="D21" s="50"/>
       <c r="E21" t="s">
         <v>3</v>
@@ -2874,7 +2874,7 @@
       <c r="M21" s="62"/>
     </row>
     <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
+      <c r="A22" s="158"/>
       <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
@@ -2939,7 +2939,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="144"/>
+      <c r="A24" s="163"/>
       <c r="B24" s="3" t="s">
         <v>57</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="L24" s="116"/>
     </row>
     <row r="25" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="142" t="s">
+      <c r="A25" s="157" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -2989,7 +2989,7 @@
       <c r="T25" s="31"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
+      <c r="A26" s="158"/>
       <c r="D26" s="50"/>
       <c r="E26" t="s">
         <v>45</v>
@@ -3006,7 +3006,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
+      <c r="A27" s="158"/>
       <c r="D27" s="50"/>
       <c r="E27" t="s">
         <v>46</v>
@@ -3023,7 +3023,7 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="143"/>
+      <c r="A28" s="158"/>
       <c r="D28" s="50"/>
       <c r="E28" t="s">
         <v>48</v>
@@ -3040,7 +3040,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="144"/>
+      <c r="A29" s="163"/>
       <c r="D29" s="50"/>
       <c r="E29" t="s">
         <v>49</v>
@@ -3140,7 +3140,7 @@
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D33" s="145" t="s">
+      <c r="D33" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E33" t="s">
@@ -3155,7 +3155,7 @@
       <c r="H33" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L33" s="138" t="s">
+      <c r="L33" s="150" t="s">
         <v>173</v>
       </c>
       <c r="M33" s="57" t="s">
@@ -3163,17 +3163,17 @@
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="146"/>
+      <c r="D34" s="153"/>
       <c r="E34" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="138"/>
+      <c r="L34" s="150"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="145" t="s">
+      <c r="D35" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
@@ -3188,20 +3188,20 @@
       <c r="H35" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="138"/>
+      <c r="L35" s="150"/>
       <c r="M35" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="146"/>
+      <c r="D36" s="153"/>
       <c r="E36" t="s">
         <v>91</v>
       </c>
       <c r="F36" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="139"/>
+      <c r="L36" s="154"/>
     </row>
     <row r="37" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
@@ -3240,7 +3240,7 @@
       <c r="T37" s="31"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="145" t="s">
+      <c r="D38" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -3255,7 +3255,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="138" t="s">
+      <c r="L38" s="150" t="s">
         <v>173</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -3263,7 +3263,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="146"/>
+      <c r="D39" s="153"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -3271,10 +3271,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="138"/>
+      <c r="L39" s="150"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="145" t="s">
+      <c r="D40" s="152" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -3292,7 +3292,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="138" t="s">
+      <c r="L40" s="150" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -3300,14 +3300,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="146"/>
+      <c r="D41" s="153"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="139"/>
+      <c r="L41" s="154"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -3366,7 +3366,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="145" t="s">
+      <c r="D44" s="152" t="s">
         <v>73</v>
       </c>
       <c r="E44" t="s">
@@ -3384,7 +3384,7 @@
       <c r="I44" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L44" s="138" t="s">
+      <c r="L44" s="150" t="s">
         <v>103</v>
       </c>
       <c r="M44" s="57" t="s">
@@ -3392,17 +3392,17 @@
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="146"/>
+      <c r="D45" s="153"/>
       <c r="E45" t="s">
         <v>91</v>
       </c>
       <c r="F45" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L45" s="138"/>
+      <c r="L45" s="150"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D46" s="145" t="s">
+      <c r="D46" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E46" t="s">
@@ -3414,7 +3414,7 @@
       <c r="G46" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="L46" s="152" t="s">
+      <c r="L46" s="155" t="s">
         <v>175</v>
       </c>
       <c r="M46" s="57" t="s">
@@ -3422,14 +3422,14 @@
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="153"/>
+      <c r="D47" s="156"/>
       <c r="E47" t="s">
         <v>127</v>
       </c>
       <c r="F47" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="L47" s="139"/>
+      <c r="L47" s="154"/>
       <c r="M47" s="57" t="s">
         <v>171</v>
       </c>
@@ -3493,7 +3493,7 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="145" t="s">
+      <c r="D50" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E50" s="42" t="s">
@@ -3505,7 +3505,7 @@
       <c r="G50" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="152" t="s">
+      <c r="L50" s="155" t="s">
         <v>175</v>
       </c>
       <c r="M50" s="57" t="s">
@@ -3513,14 +3513,14 @@
       </c>
     </row>
     <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="146"/>
+      <c r="D51" s="153"/>
       <c r="E51" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F51" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="139"/>
+      <c r="L51" s="154"/>
       <c r="M51" s="57" t="s">
         <v>152</v>
       </c>
@@ -3578,7 +3578,7 @@
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="145" t="s">
+      <c r="D54" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E54" t="s">
@@ -3593,7 +3593,7 @@
       <c r="H54" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="138" t="s">
+      <c r="L54" s="150" t="s">
         <v>162</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -3601,7 +3601,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="146"/>
+      <c r="D55" s="153"/>
       <c r="E55" t="s">
         <v>150</v>
       </c>
@@ -3614,7 +3614,7 @@
       <c r="H55" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="139"/>
+      <c r="L55" s="154"/>
       <c r="M55" s="57" t="s">
         <v>169</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="140" t="s">
+      <c r="D58" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -3688,7 +3688,7 @@
       <c r="G58" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="L58" s="138" t="s">
+      <c r="L58" s="150" t="s">
         <v>167</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -3696,7 +3696,7 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="141"/>
+      <c r="D59" s="165"/>
       <c r="E59" s="42" t="s">
         <v>164</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="G59" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="L59" s="139"/>
+      <c r="L59" s="154"/>
       <c r="M59" s="57" t="s">
         <v>166</v>
       </c>
@@ -3730,6 +3730,21 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="D50:D51"/>
@@ -3744,21 +3759,6 @@
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="L7:L8"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="L58:L59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D44:D45"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3794,23 +3794,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="154" t="s">
+      <c r="F1" s="166" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="156"/>
-      <c r="N1" s="154" t="s">
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="168"/>
+      <c r="N1" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="155"/>
-      <c r="P1" s="155"/>
-      <c r="Q1" s="155"/>
-      <c r="R1" s="156"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="168"/>
     </row>
     <row r="2" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="157" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -3865,7 +3865,7 @@
       <c r="AA2" s="31"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="143"/>
+      <c r="A3" s="158"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="143"/>
+      <c r="A4" s="158"/>
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -3909,7 +3909,7 @@
       <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -3963,7 +3963,7 @@
       <c r="AA5" s="10"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="143"/>
+      <c r="A6" s="158"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -3987,13 +3987,13 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="144"/>
+      <c r="A7" s="163"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142" t="s">
+      <c r="A8" s="157" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4043,7 +4043,7 @@
       <c r="AA8" s="31"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="144"/>
+      <c r="A9" s="163"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -4070,7 +4070,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="142" t="s">
+      <c r="A10" s="157" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -4114,7 +4114,7 @@
       <c r="AA10" s="31"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="143"/>
+      <c r="A11" s="158"/>
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4132,7 +4132,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
+      <c r="A12" s="158"/>
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -4144,13 +4144,13 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
+      <c r="A13" s="158"/>
       <c r="T13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -4194,7 +4194,7 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -4221,7 +4221,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
+      <c r="A16" s="158"/>
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -4230,7 +4230,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
@@ -4301,7 +4301,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="144"/>
+      <c r="A19" s="163"/>
       <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="142" t="s">
+      <c r="A20" s="157" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4352,7 +4352,7 @@
       <c r="AA20" s="31"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
+      <c r="A21" s="158"/>
       <c r="D21" t="s">
         <v>4</v>
       </c>
@@ -4367,7 +4367,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
+      <c r="A22" s="158"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
@@ -4382,7 +4382,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
+      <c r="A23" s="158"/>
       <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
@@ -4419,7 +4419,7 @@
       <c r="AA23" s="10"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
+      <c r="A24" s="158"/>
       <c r="D24" t="s">
         <v>45</v>
       </c>
@@ -4434,7 +4434,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
+      <c r="A25" s="158"/>
       <c r="D25" t="s">
         <v>46</v>
       </c>
@@ -4449,7 +4449,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
+      <c r="A26" s="158"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -4464,7 +4464,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="144"/>
+      <c r="A27" s="163"/>
       <c r="D27" t="s">
         <v>49</v>
       </c>
@@ -4601,14 +4601,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="148" t="s">
+      <c r="F1" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -4617,7 +4617,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="157" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -4626,7 +4626,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="142" t="s">
+      <c r="D2" s="157" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -4659,8 +4659,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="143"/>
-      <c r="D3" s="143"/>
+      <c r="A3" s="158"/>
+      <c r="D3" s="158"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -4673,7 +4673,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="138" t="s">
+      <c r="L3" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -4681,8 +4681,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="143"/>
-      <c r="D4" s="150"/>
+      <c r="A4" s="158"/>
+      <c r="D4" s="159"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -4699,14 +4699,14 @@
       </c>
     </row>
     <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="147" t="s">
+      <c r="D5" s="162" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4739,8 +4739,8 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="143"/>
-      <c r="D6" s="143"/>
+      <c r="A6" s="158"/>
+      <c r="D6" s="158"/>
       <c r="E6" t="s">
         <v>2</v>
       </c>
@@ -4753,7 +4753,7 @@
       <c r="H6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="138" t="s">
+      <c r="L6" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="57" t="s">
@@ -4761,8 +4761,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="144"/>
-      <c r="D7" s="144"/>
+      <c r="A7" s="163"/>
+      <c r="D7" s="163"/>
       <c r="E7" t="s">
         <v>3</v>
       </c>
@@ -4772,7 +4772,7 @@
       <c r="L7" s="151"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142" t="s">
+      <c r="A8" s="157" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4781,7 +4781,7 @@
       <c r="C8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="142" t="s">
+      <c r="D8" s="157" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4812,11 +4812,11 @@
       <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
+      <c r="A9" s="158"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="143"/>
+      <c r="D9" s="158"/>
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -4835,10 +4835,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
+      <c r="A10" s="158"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
-      <c r="D10" s="147" t="s">
+      <c r="D10" s="162" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -4867,8 +4867,8 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144"/>
-      <c r="D11" s="144"/>
+      <c r="A11" s="163"/>
+      <c r="D11" s="163"/>
       <c r="E11" t="s">
         <v>16</v>
       </c>
@@ -4888,7 +4888,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="142" t="s">
+      <c r="A12" s="157" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -4926,7 +4926,7 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
+      <c r="A13" s="158"/>
       <c r="D13" s="50"/>
       <c r="E13" t="s">
         <v>21</v>
@@ -4946,7 +4946,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
+      <c r="A14" s="158"/>
       <c r="D14" s="52"/>
       <c r="E14" s="53" t="s">
         <v>3</v>
@@ -4970,7 +4970,7 @@
       <c r="T14" s="56"/>
     </row>
     <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
@@ -5006,7 +5006,7 @@
       <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
+      <c r="A16" s="158"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
@@ -5032,7 +5032,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
+      <c r="A17" s="158"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>3</v>
@@ -5044,7 +5044,7 @@
       <c r="M17" s="62"/>
     </row>
     <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
@@ -5080,7 +5080,7 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
+      <c r="A19" s="158"/>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
@@ -5109,7 +5109,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="144"/>
+      <c r="A20" s="163"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -5123,7 +5123,7 @@
       <c r="L20" s="116"/>
     </row>
     <row r="21" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="142" t="s">
+      <c r="A21" s="157" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -5159,7 +5159,7 @@
       <c r="T21" s="31"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
+      <c r="A22" s="158"/>
       <c r="D22" s="50"/>
       <c r="E22" t="s">
         <v>45</v>
@@ -5176,7 +5176,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
+      <c r="A23" s="158"/>
       <c r="D23" s="50"/>
       <c r="E23" t="s">
         <v>46</v>
@@ -5193,7 +5193,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
+      <c r="A24" s="158"/>
       <c r="D24" s="50"/>
       <c r="E24" t="s">
         <v>48</v>
@@ -5210,7 +5210,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="144"/>
+      <c r="A25" s="163"/>
       <c r="D25" s="50"/>
       <c r="E25" t="s">
         <v>49</v>
@@ -5310,7 +5310,7 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="145" t="s">
+      <c r="D29" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
@@ -5325,7 +5325,7 @@
       <c r="H29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="138" t="s">
+      <c r="L29" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M29" s="57" t="s">
@@ -5333,7 +5333,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="146"/>
+      <c r="D30" s="153"/>
       <c r="E30" t="s">
         <v>4</v>
       </c>
@@ -5343,10 +5343,10 @@
       <c r="G30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="138"/>
+      <c r="L30" s="150"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="145" t="s">
+      <c r="D31" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
@@ -5361,13 +5361,13 @@
       <c r="H31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="138"/>
+      <c r="L31" s="150"/>
       <c r="M31" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="146"/>
+      <c r="D32" s="153"/>
       <c r="E32" t="s">
         <v>49</v>
       </c>
@@ -5377,7 +5377,7 @@
       <c r="G32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L32" s="139"/>
+      <c r="L32" s="154"/>
     </row>
     <row r="33" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
@@ -5435,7 +5435,7 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="145" t="s">
+      <c r="D35" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -5450,7 +5450,7 @@
       <c r="H35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="138" t="s">
+      <c r="L35" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="57" t="s">
@@ -5458,7 +5458,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="159"/>
+      <c r="D36" s="169"/>
       <c r="E36" s="43" t="s">
         <v>3</v>
       </c>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="G36" s="46"/>
       <c r="H36" s="65"/>
-      <c r="L36" s="158"/>
+      <c r="L36" s="170"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D37" s="70" t="s">
@@ -5496,7 +5496,7 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="145" t="s">
+      <c r="D38" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -5511,7 +5511,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="138" t="s">
+      <c r="L38" s="150" t="s">
         <v>131</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -5519,7 +5519,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="146"/>
+      <c r="D39" s="153"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -5527,10 +5527,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="138"/>
+      <c r="L39" s="150"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="145" t="s">
+      <c r="D40" s="152" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -5548,7 +5548,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="138" t="s">
+      <c r="L40" s="150" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -5556,14 +5556,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="146"/>
+      <c r="D41" s="153"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="139"/>
+      <c r="L41" s="154"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -5605,7 +5605,7 @@
       <c r="T42" s="31"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="145" t="s">
+      <c r="D43" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
@@ -5620,7 +5620,7 @@
       <c r="H43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="138" t="s">
+      <c r="L43" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -5628,7 +5628,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="146"/>
+      <c r="D44" s="153"/>
       <c r="E44" t="s">
         <v>124</v>
       </c>
@@ -5638,13 +5638,13 @@
       <c r="G44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="138"/>
+      <c r="L44" s="150"/>
       <c r="M44" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="145" t="s">
+      <c r="D45" s="152" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -5662,7 +5662,7 @@
       <c r="I45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="138" t="s">
+      <c r="L45" s="150" t="s">
         <v>103</v>
       </c>
       <c r="M45" s="57" t="s">
@@ -5670,14 +5670,14 @@
       </c>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="159"/>
+      <c r="D46" s="169"/>
       <c r="E46" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L46" s="158"/>
+      <c r="L46" s="170"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D47" s="70" t="s">
@@ -5726,7 +5726,7 @@
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="145" t="s">
+      <c r="D49" s="152" t="s">
         <v>73</v>
       </c>
       <c r="E49" t="s">
@@ -5744,7 +5744,7 @@
       <c r="I49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="138" t="s">
+      <c r="L49" s="150" t="s">
         <v>103</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -5752,17 +5752,17 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="146"/>
+      <c r="D50" s="153"/>
       <c r="E50" t="s">
         <v>91</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="138"/>
+      <c r="L50" s="150"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D51" s="145" t="s">
+      <c r="D51" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E51" t="s">
@@ -5774,7 +5774,7 @@
       <c r="G51" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L51" s="152" t="s">
+      <c r="L51" s="155" t="s">
         <v>158</v>
       </c>
       <c r="M51" s="57" t="s">
@@ -5782,14 +5782,14 @@
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="153"/>
+      <c r="D52" s="156"/>
       <c r="E52" t="s">
         <v>127</v>
       </c>
       <c r="F52" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="139"/>
+      <c r="L52" s="154"/>
       <c r="M52" s="57" t="s">
         <v>154</v>
       </c>
@@ -5836,7 +5836,7 @@
       <c r="T53" s="31"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="145" t="s">
+      <c r="D54" s="152" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="42" t="s">
@@ -5851,7 +5851,7 @@
       <c r="H54" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="138" t="s">
+      <c r="L54" s="150" t="s">
         <v>102</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -5859,7 +5859,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="157"/>
+      <c r="D55" s="171"/>
       <c r="E55" s="42" t="s">
         <v>4</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>19</v>
       </c>
       <c r="H55" s="46"/>
-      <c r="L55" s="158"/>
+      <c r="L55" s="170"/>
       <c r="M55" s="57" t="s">
         <v>152</v>
       </c>
@@ -5924,7 +5924,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="145" t="s">
+      <c r="D58" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -5936,7 +5936,7 @@
       <c r="G58" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="152" t="s">
+      <c r="L58" s="155" t="s">
         <v>158</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -5944,14 +5944,14 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="146"/>
+      <c r="D59" s="153"/>
       <c r="E59" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F59" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="139"/>
+      <c r="L59" s="154"/>
       <c r="M59" s="57" t="s">
         <v>152</v>
       </c>
@@ -6075,7 +6075,7 @@
       </c>
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D65" s="145" t="s">
+      <c r="D65" s="152" t="s">
         <v>74</v>
       </c>
       <c r="E65" t="s">
@@ -6090,7 +6090,7 @@
       <c r="H65" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L65" s="138" t="s">
+      <c r="L65" s="150" t="s">
         <v>162</v>
       </c>
       <c r="M65" s="57" t="s">
@@ -6098,7 +6098,7 @@
       </c>
     </row>
     <row r="66" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="146"/>
+      <c r="D66" s="153"/>
       <c r="E66" t="s">
         <v>150</v>
       </c>
@@ -6111,7 +6111,7 @@
       <c r="H66" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L66" s="139"/>
+      <c r="L66" s="154"/>
       <c r="M66" s="57" t="s">
         <v>147</v>
       </c>
@@ -6135,30 +6135,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="L45:L46"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D65:D66"/>
@@ -6169,6 +6145,30 @@
     <mergeCell ref="L51:L52"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L54:L55"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
keep exit deeper in the stack than loop for r-form right recursion
We want the last items first, as a LL(1). We can either
- ops = [loop nt, exit f], and deliver all the public exit() in the reverse order on the last iteration (non-looping factor)
- ops = [exit f, enter nt], and deliver the public exit() naturally

The 2nd solution is simpler, though it's a little costlier on the stacks (parser stack + wrapper stack instead of just wrapper stack)
</commit_message>
<xml_diff>
--- a/doc/ops.xlsx
+++ b/doc/ops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="185">
   <si>
     <t>A → α β+ γ</t>
   </si>
@@ -987,9 +987,6 @@
 |parent_fact</t>
   </si>
   <si>
-    <t>exit_A → does nothing; enter_A → pushes priority p(0) on asm_stack</t>
-  </si>
-  <si>
     <t>child_fact(A)
 |parent_fact</t>
   </si>
@@ -1003,6 +1000,12 @@
   <si>
     <t>L|r_rec
 |parent_fact</t>
+  </si>
+  <si>
+    <t>L|r_rec</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={α})</t>
   </si>
 </sst>
 </file>
@@ -1953,95 +1956,95 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2349,7 +2352,9 @@
   </sheetPr>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2373,14 +2378,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="158" t="s">
+      <c r="F1" s="163" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
+      <c r="I1" s="164"/>
+      <c r="J1" s="164"/>
+      <c r="K1" s="164"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -2389,7 +2394,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -2398,7 +2403,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="152" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -2431,8 +2436,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="152"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="153"/>
+      <c r="D3" s="153"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -2445,7 +2450,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="154" t="s">
+      <c r="L3" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -2453,8 +2458,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="D4" s="152"/>
+      <c r="A4" s="153"/>
+      <c r="D4" s="153"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -2465,17 +2470,17 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="154"/>
+      <c r="L4" s="151"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="143" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="143" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="143" t="s">
         <v>1</v>
       </c>
@@ -2506,8 +2511,8 @@
       <c r="T5" s="148"/>
     </row>
     <row r="6" spans="1:20" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="152"/>
-      <c r="D6" s="152"/>
+      <c r="A6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="138" t="s">
         <v>45</v>
       </c>
@@ -2527,8 +2532,8 @@
       <c r="M6" s="140"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="152"/>
-      <c r="D7" s="152"/>
+      <c r="A7" s="153"/>
+      <c r="D7" s="153"/>
       <c r="E7" s="42" t="s">
         <v>139</v>
       </c>
@@ -2542,7 +2547,7 @@
       <c r="I7" s="46"/>
       <c r="J7" s="46"/>
       <c r="K7" s="46"/>
-      <c r="L7" s="154" t="s">
+      <c r="L7" s="151" t="s">
         <v>174</v>
       </c>
       <c r="M7" s="57" t="s">
@@ -2550,8 +2555,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="152"/>
-      <c r="D8" s="153"/>
+      <c r="A8" s="153"/>
+      <c r="D8" s="172"/>
       <c r="E8" s="42" t="s">
         <v>91</v>
       </c>
@@ -2563,17 +2568,17 @@
       <c r="I8" s="46"/>
       <c r="J8" s="46"/>
       <c r="K8" s="46"/>
-      <c r="L8" s="155"/>
+      <c r="L8" s="161"/>
     </row>
     <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="152"/>
+      <c r="A9" s="153"/>
       <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="161" t="s">
+      <c r="D9" s="155" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -2606,8 +2611,8 @@
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
-      <c r="D10" s="152"/>
+      <c r="A10" s="153"/>
+      <c r="D10" s="153"/>
       <c r="E10" t="s">
         <v>2</v>
       </c>
@@ -2620,7 +2625,7 @@
       <c r="H10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="154" t="s">
+      <c r="L10" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M10" s="57" t="s">
@@ -2628,18 +2633,18 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="162"/>
-      <c r="D11" s="162"/>
+      <c r="A11" s="154"/>
+      <c r="D11" s="154"/>
       <c r="E11" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="155"/>
+      <c r="L11" s="161"/>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -2648,7 +2653,7 @@
       <c r="C12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="151" t="s">
+      <c r="D12" s="152" t="s">
         <v>81</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -2666,8 +2671,8 @@
       <c r="I12" s="36"/>
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
-      <c r="L12" s="171" t="s">
-        <v>181</v>
+      <c r="L12" s="165" t="s">
+        <v>183</v>
       </c>
       <c r="M12" s="60" t="s">
         <v>85</v>
@@ -2681,11 +2686,11 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="152"/>
+      <c r="A13" s="153"/>
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="152"/>
+      <c r="D13" s="153"/>
       <c r="E13" t="s">
         <v>16</v>
       </c>
@@ -2698,26 +2703,26 @@
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
-      <c r="L13" s="172"/>
+      <c r="L13" s="166"/>
       <c r="M13" s="57" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="43"/>
       <c r="C14" s="43"/>
-      <c r="D14" s="161" t="s">
+      <c r="D14" s="155" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>18</v>
@@ -2725,11 +2730,11 @@
       <c r="I14" s="49"/>
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
-      <c r="L14" s="173" t="s">
-        <v>181</v>
+      <c r="L14" s="167" t="s">
+        <v>180</v>
       </c>
       <c r="M14" s="59" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2740,8 +2745,8 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="162"/>
-      <c r="D15" s="162"/>
+      <c r="A15" s="154"/>
+      <c r="D15" s="154"/>
       <c r="E15" t="s">
         <v>16</v>
       </c>
@@ -2755,13 +2760,13 @@
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="174"/>
+      <c r="L15" s="168"/>
       <c r="M15" s="57" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -2799,7 +2804,7 @@
       <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="152"/>
+      <c r="A17" s="153"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>21</v>
@@ -2813,7 +2818,7 @@
       <c r="H17" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="154" t="s">
+      <c r="L17" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M17" s="57" t="s">
@@ -2821,7 +2826,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="152"/>
+      <c r="A18" s="153"/>
       <c r="D18" s="52"/>
       <c r="E18" s="53" t="s">
         <v>3</v>
@@ -2834,7 +2839,7 @@
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="155"/>
+      <c r="L18" s="161"/>
       <c r="M18" s="61"/>
       <c r="N18" s="56"/>
       <c r="O18" s="56"/>
@@ -2845,7 +2850,7 @@
       <c r="T18" s="56"/>
     </row>
     <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2881,7 +2886,7 @@
       <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="152"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
@@ -2901,15 +2906,15 @@
       <c r="I20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="157" t="s">
-        <v>182</v>
+      <c r="L20" s="162" t="s">
+        <v>181</v>
       </c>
       <c r="M20" s="62" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="153"/>
       <c r="D21" s="50"/>
       <c r="E21" t="s">
         <v>3</v>
@@ -2917,11 +2922,11 @@
       <c r="F21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="155"/>
+      <c r="L21" s="161"/>
       <c r="M21" s="62"/>
     </row>
     <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
@@ -2957,7 +2962,7 @@
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
@@ -2980,7 +2985,7 @@
       <c r="J23" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="154" t="s">
+      <c r="L23" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M23" s="62" t="s">
@@ -2988,7 +2993,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="162"/>
+      <c r="A24" s="154"/>
       <c r="B24" s="3" t="s">
         <v>57</v>
       </c>
@@ -3002,7 +3007,7 @@
       <c r="L24" s="156"/>
     </row>
     <row r="25" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="151" t="s">
+      <c r="A25" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -3040,7 +3045,7 @@
       <c r="T25" s="31"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="152"/>
+      <c r="A26" s="153"/>
       <c r="D26" s="50"/>
       <c r="E26" t="s">
         <v>45</v>
@@ -3051,15 +3056,15 @@
       <c r="G26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="157" t="s">
-        <v>180</v>
+      <c r="L26" s="162" t="s">
+        <v>179</v>
       </c>
       <c r="M26" s="64" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="152"/>
+      <c r="A27" s="153"/>
       <c r="D27" s="50"/>
       <c r="E27" t="s">
         <v>46</v>
@@ -3070,13 +3075,13 @@
       <c r="G27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L27" s="154"/>
+      <c r="L27" s="151"/>
       <c r="M27" s="57" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="152"/>
+      <c r="A28" s="153"/>
       <c r="D28" s="50"/>
       <c r="E28" t="s">
         <v>48</v>
@@ -3087,7 +3092,7 @@
       <c r="G28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="154" t="s">
+      <c r="L28" s="151" t="s">
         <v>174</v>
       </c>
       <c r="M28" s="57" t="s">
@@ -3095,7 +3100,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="162"/>
+      <c r="A29" s="154"/>
       <c r="D29" s="50"/>
       <c r="E29" t="s">
         <v>49</v>
@@ -3195,7 +3200,7 @@
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D33" s="149" t="s">
+      <c r="D33" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E33" t="s">
@@ -3210,7 +3215,7 @@
       <c r="H33" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L33" s="154" t="s">
+      <c r="L33" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M33" s="57" t="s">
@@ -3225,10 +3230,10 @@
       <c r="F34" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="154"/>
+      <c r="L34" s="151"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="149" t="s">
+      <c r="D35" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
@@ -3243,7 +3248,7 @@
       <c r="H35" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="154"/>
+      <c r="L35" s="151"/>
       <c r="M35" s="57" t="s">
         <v>151</v>
       </c>
@@ -3295,7 +3300,7 @@
       <c r="T37" s="31"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="149" t="s">
+      <c r="D38" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -3310,7 +3315,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="154" t="s">
+      <c r="L38" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -3326,10 +3331,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="154"/>
+      <c r="L39" s="151"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="149" t="s">
+      <c r="D40" s="159" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -3347,7 +3352,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="154" t="s">
+      <c r="L40" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -3413,7 +3418,7 @@
       <c r="G43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="175" t="s">
+      <c r="L43" s="149" t="s">
         <v>160</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -3421,7 +3426,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="149" t="s">
+      <c r="D44" s="159" t="s">
         <v>73</v>
       </c>
       <c r="E44" t="s">
@@ -3439,7 +3444,7 @@
       <c r="I44" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L44" s="154" t="s">
+      <c r="L44" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M44" s="57" t="s">
@@ -3454,10 +3459,10 @@
       <c r="F45" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L45" s="154"/>
+      <c r="L45" s="151"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D46" s="149" t="s">
+      <c r="D46" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E46" t="s">
@@ -3469,7 +3474,7 @@
       <c r="G46" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="L46" s="157" t="s">
+      <c r="L46" s="162" t="s">
         <v>175</v>
       </c>
       <c r="M46" s="57" t="s">
@@ -3477,7 +3482,7 @@
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="150"/>
+      <c r="D47" s="171"/>
       <c r="E47" t="s">
         <v>127</v>
       </c>
@@ -3540,7 +3545,7 @@
       <c r="G49" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L49" s="175" t="s">
+      <c r="L49" s="149" t="s">
         <v>160</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -3548,7 +3553,7 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="149" t="s">
+      <c r="D50" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E50" s="42" t="s">
@@ -3560,7 +3565,7 @@
       <c r="G50" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="157" t="s">
+      <c r="L50" s="162" t="s">
         <v>175</v>
       </c>
       <c r="M50" s="57" t="s">
@@ -3603,8 +3608,8 @@
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
-      <c r="L52" s="177" t="s">
-        <v>183</v>
+      <c r="L52" s="169" t="s">
+        <v>182</v>
       </c>
       <c r="M52" s="60" t="s">
         <v>156</v>
@@ -3627,13 +3632,13 @@
       <c r="G53" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L53" s="176"/>
+      <c r="L53" s="170"/>
       <c r="M53" s="57" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="149" t="s">
+      <c r="D54" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E54" t="s">
@@ -3648,7 +3653,7 @@
       <c r="H54" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="154" t="s">
+      <c r="L54" s="151" t="s">
         <v>167</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -3699,8 +3704,8 @@
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
-      <c r="L56" s="178" t="s">
-        <v>183</v>
+      <c r="L56" s="150" t="s">
+        <v>182</v>
       </c>
       <c r="M56" s="60" t="s">
         <v>85</v>
@@ -3723,13 +3728,13 @@
       <c r="G57" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="154"/>
+      <c r="L57" s="151"/>
       <c r="M57" s="57" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="163" t="s">
+      <c r="D58" s="157" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -3741,7 +3746,7 @@
       <c r="G58" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="L58" s="154" t="s">
+      <c r="L58" s="151" t="s">
         <v>167</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -3749,7 +3754,7 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="164"/>
+      <c r="D59" s="158"/>
       <c r="E59" s="42" t="s">
         <v>164</v>
       </c>
@@ -3783,40 +3788,40 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="L56:L57"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D2:D8"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="D44:D45"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L10:L11"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L33:L36"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="L50:L51"/>
     <mergeCell ref="L54:L55"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="L26:L27"/>
     <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="L56:L57"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L10:L11"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L20:L21"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="L52:L53"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D2:D8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="L40:L41"/>
     <mergeCell ref="L44:L45"/>
@@ -3856,23 +3861,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="165" t="s">
+      <c r="F1" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="167"/>
-      <c r="N1" s="165" t="s">
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
+      <c r="J1" s="175"/>
+      <c r="N1" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="167"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="175"/>
     </row>
     <row r="2" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -3927,7 +3932,7 @@
       <c r="AA2" s="31"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="152"/>
+      <c r="A3" s="153"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -3951,7 +3956,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
+      <c r="A4" s="153"/>
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -3971,7 +3976,7 @@
       <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -4025,7 +4030,7 @@
       <c r="AA5" s="10"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="152"/>
+      <c r="A6" s="153"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -4049,13 +4054,13 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="162"/>
+      <c r="A7" s="154"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4105,7 +4110,7 @@
       <c r="AA8" s="31"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="162"/>
+      <c r="A9" s="154"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -4132,7 +4137,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -4176,7 +4181,7 @@
       <c r="AA10" s="31"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="152"/>
+      <c r="A11" s="153"/>
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4194,7 +4199,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="153"/>
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -4206,13 +4211,13 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="152"/>
+      <c r="A13" s="153"/>
       <c r="T13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -4256,7 +4261,7 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="152"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -4283,7 +4288,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="152"/>
+      <c r="A16" s="153"/>
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -4292,7 +4297,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="152"/>
+      <c r="A17" s="153"/>
       <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4336,7 +4341,7 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="152"/>
+      <c r="A18" s="153"/>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
@@ -4363,7 +4368,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="162"/>
+      <c r="A19" s="154"/>
       <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
@@ -4372,7 +4377,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4414,7 +4419,7 @@
       <c r="AA20" s="31"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="153"/>
       <c r="D21" t="s">
         <v>4</v>
       </c>
@@ -4429,7 +4434,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
@@ -4444,7 +4449,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
@@ -4481,7 +4486,7 @@
       <c r="AA23" s="10"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
+      <c r="A24" s="153"/>
       <c r="D24" t="s">
         <v>45</v>
       </c>
@@ -4496,7 +4501,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="152"/>
+      <c r="A25" s="153"/>
       <c r="D25" t="s">
         <v>46</v>
       </c>
@@ -4511,7 +4516,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="152"/>
+      <c r="A26" s="153"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -4526,7 +4531,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="162"/>
+      <c r="A27" s="154"/>
       <c r="D27" t="s">
         <v>49</v>
       </c>
@@ -4663,14 +4668,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="158" t="s">
+      <c r="F1" s="163" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
+      <c r="I1" s="164"/>
+      <c r="J1" s="164"/>
+      <c r="K1" s="164"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -4679,7 +4684,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -4688,7 +4693,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="152" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -4721,8 +4726,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="152"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="153"/>
+      <c r="D3" s="153"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -4735,7 +4740,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="154" t="s">
+      <c r="L3" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -4743,8 +4748,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="D4" s="153"/>
+      <c r="A4" s="153"/>
+      <c r="D4" s="172"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -4755,20 +4760,20 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="155"/>
+      <c r="L4" s="161"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="155" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4801,8 +4806,8 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="152"/>
-      <c r="D6" s="152"/>
+      <c r="A6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="E6" t="s">
         <v>2</v>
       </c>
@@ -4815,7 +4820,7 @@
       <c r="H6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="154" t="s">
+      <c r="L6" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="57" t="s">
@@ -4823,18 +4828,18 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="162"/>
-      <c r="D7" s="162"/>
+      <c r="A7" s="154"/>
+      <c r="D7" s="154"/>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="155"/>
+      <c r="L7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4843,7 +4848,7 @@
       <c r="C8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="152" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4874,11 +4879,11 @@
       <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="152"/>
+      <c r="A9" s="153"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="152"/>
+      <c r="D9" s="153"/>
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -4897,10 +4902,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
-      <c r="D10" s="161" t="s">
+      <c r="D10" s="155" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -4929,8 +4934,8 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="162"/>
-      <c r="D11" s="162"/>
+      <c r="A11" s="154"/>
+      <c r="D11" s="154"/>
       <c r="E11" t="s">
         <v>16</v>
       </c>
@@ -4950,7 +4955,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -4988,7 +4993,7 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="152"/>
+      <c r="A13" s="153"/>
       <c r="D13" s="50"/>
       <c r="E13" t="s">
         <v>21</v>
@@ -5008,7 +5013,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
+      <c r="A14" s="153"/>
       <c r="D14" s="52"/>
       <c r="E14" s="53" t="s">
         <v>3</v>
@@ -5032,7 +5037,7 @@
       <c r="T14" s="56"/>
     </row>
     <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="152"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
@@ -5068,7 +5073,7 @@
       <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="152"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
@@ -5094,7 +5099,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="152"/>
+      <c r="A17" s="153"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>3</v>
@@ -5106,7 +5111,7 @@
       <c r="M17" s="62"/>
     </row>
     <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="152"/>
+      <c r="A18" s="153"/>
       <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
@@ -5142,7 +5147,7 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
@@ -5171,7 +5176,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="162"/>
+      <c r="A20" s="154"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -5185,7 +5190,7 @@
       <c r="L20" s="116"/>
     </row>
     <row r="21" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="151" t="s">
+      <c r="A21" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -5221,7 +5226,7 @@
       <c r="T21" s="31"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="D22" s="50"/>
       <c r="E22" t="s">
         <v>45</v>
@@ -5238,7 +5243,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="D23" s="50"/>
       <c r="E23" t="s">
         <v>46</v>
@@ -5255,7 +5260,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
+      <c r="A24" s="153"/>
       <c r="D24" s="50"/>
       <c r="E24" t="s">
         <v>48</v>
@@ -5272,7 +5277,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="162"/>
+      <c r="A25" s="154"/>
       <c r="D25" s="50"/>
       <c r="E25" t="s">
         <v>49</v>
@@ -5372,7 +5377,7 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="149" t="s">
+      <c r="D29" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
@@ -5387,7 +5392,7 @@
       <c r="H29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="154" t="s">
+      <c r="L29" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M29" s="57" t="s">
@@ -5405,10 +5410,10 @@
       <c r="G30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="154"/>
+      <c r="L30" s="151"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="149" t="s">
+      <c r="D31" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
@@ -5423,7 +5428,7 @@
       <c r="H31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="154"/>
+      <c r="L31" s="151"/>
       <c r="M31" s="57" t="s">
         <v>151</v>
       </c>
@@ -5497,7 +5502,7 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="149" t="s">
+      <c r="D35" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -5512,7 +5517,7 @@
       <c r="H35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="154" t="s">
+      <c r="L35" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="57" t="s">
@@ -5520,7 +5525,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="168"/>
+      <c r="D36" s="178"/>
       <c r="E36" s="43" t="s">
         <v>3</v>
       </c>
@@ -5529,7 +5534,7 @@
       </c>
       <c r="G36" s="46"/>
       <c r="H36" s="65"/>
-      <c r="L36" s="169"/>
+      <c r="L36" s="177"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D37" s="70" t="s">
@@ -5558,7 +5563,7 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="149" t="s">
+      <c r="D38" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -5573,7 +5578,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="154" t="s">
+      <c r="L38" s="151" t="s">
         <v>131</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -5589,10 +5594,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="154"/>
+      <c r="L39" s="151"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="149" t="s">
+      <c r="D40" s="159" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -5610,7 +5615,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="154" t="s">
+      <c r="L40" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -5667,7 +5672,7 @@
       <c r="T42" s="31"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="149" t="s">
+      <c r="D43" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
@@ -5682,7 +5687,7 @@
       <c r="H43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="154" t="s">
+      <c r="L43" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -5700,13 +5705,13 @@
       <c r="G44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="154"/>
+      <c r="L44" s="151"/>
       <c r="M44" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="149" t="s">
+      <c r="D45" s="159" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -5724,7 +5729,7 @@
       <c r="I45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="154" t="s">
+      <c r="L45" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M45" s="57" t="s">
@@ -5732,14 +5737,14 @@
       </c>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="168"/>
+      <c r="D46" s="178"/>
       <c r="E46" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L46" s="169"/>
+      <c r="L46" s="177"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D47" s="70" t="s">
@@ -5788,7 +5793,7 @@
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="149" t="s">
+      <c r="D49" s="159" t="s">
         <v>73</v>
       </c>
       <c r="E49" t="s">
@@ -5806,7 +5811,7 @@
       <c r="I49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="154" t="s">
+      <c r="L49" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -5821,10 +5826,10 @@
       <c r="F50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="154"/>
+      <c r="L50" s="151"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D51" s="149" t="s">
+      <c r="D51" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E51" t="s">
@@ -5836,7 +5841,7 @@
       <c r="G51" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L51" s="157" t="s">
+      <c r="L51" s="162" t="s">
         <v>158</v>
       </c>
       <c r="M51" s="57" t="s">
@@ -5844,7 +5849,7 @@
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="150"/>
+      <c r="D52" s="171"/>
       <c r="E52" t="s">
         <v>127</v>
       </c>
@@ -5898,7 +5903,7 @@
       <c r="T53" s="31"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="149" t="s">
+      <c r="D54" s="159" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="42" t="s">
@@ -5913,7 +5918,7 @@
       <c r="H54" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="154" t="s">
+      <c r="L54" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -5921,7 +5926,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="170"/>
+      <c r="D55" s="176"/>
       <c r="E55" s="42" t="s">
         <v>4</v>
       </c>
@@ -5932,7 +5937,7 @@
         <v>19</v>
       </c>
       <c r="H55" s="46"/>
-      <c r="L55" s="169"/>
+      <c r="L55" s="177"/>
       <c r="M55" s="57" t="s">
         <v>152</v>
       </c>
@@ -5986,7 +5991,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="149" t="s">
+      <c r="D58" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -5998,7 +6003,7 @@
       <c r="G58" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="157" t="s">
+      <c r="L58" s="162" t="s">
         <v>158</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -6137,7 +6142,7 @@
       </c>
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D65" s="149" t="s">
+      <c r="D65" s="159" t="s">
         <v>74</v>
       </c>
       <c r="E65" t="s">
@@ -6152,7 +6157,7 @@
       <c r="H65" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L65" s="154" t="s">
+      <c r="L65" s="151" t="s">
         <v>162</v>
       </c>
       <c r="M65" s="57" t="s">
@@ -6197,6 +6202,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="L45:L46"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D65:D66"/>
@@ -6207,30 +6236,6 @@
     <mergeCell ref="L51:L52"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L54:L55"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
add listener & wrapper examples for star normalization (L form)
</commit_message>
<xml_diff>
--- a/doc/ops.xlsx
+++ b/doc/ops.xlsx
@@ -1999,91 +1999,91 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2392,8 +2392,8 @@
   </sheetPr>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,14 +2418,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="150" t="s">
+      <c r="F1" s="170" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="171"/>
+      <c r="K1" s="171"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -2434,7 +2434,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -2443,7 +2443,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="157" t="s">
+      <c r="D2" s="152" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -2476,8 +2476,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="155"/>
-      <c r="D3" s="155"/>
+      <c r="A3" s="153"/>
+      <c r="D3" s="153"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="159" t="s">
+      <c r="L3" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -2498,8 +2498,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
-      <c r="D4" s="155"/>
+      <c r="A4" s="153"/>
+      <c r="D4" s="153"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -2510,17 +2510,17 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="159"/>
+      <c r="L4" s="151"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="143" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="143" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="155"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="143" t="s">
         <v>1</v>
       </c>
@@ -2551,8 +2551,8 @@
       <c r="T5" s="148"/>
     </row>
     <row r="6" spans="1:20" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
-      <c r="D6" s="155"/>
+      <c r="A6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="138" t="s">
         <v>45</v>
       </c>
@@ -2572,8 +2572,8 @@
       <c r="M6" s="140"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="D7" s="155"/>
+      <c r="A7" s="153"/>
+      <c r="D7" s="153"/>
       <c r="E7" s="42" t="s">
         <v>139</v>
       </c>
@@ -2587,7 +2587,7 @@
       <c r="I7" s="46"/>
       <c r="J7" s="46"/>
       <c r="K7" s="46"/>
-      <c r="L7" s="159" t="s">
+      <c r="L7" s="151" t="s">
         <v>174</v>
       </c>
       <c r="M7" s="57" t="s">
@@ -2595,8 +2595,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="D8" s="158"/>
+      <c r="A8" s="153"/>
+      <c r="D8" s="172"/>
       <c r="E8" s="42" t="s">
         <v>91</v>
       </c>
@@ -2608,17 +2608,17 @@
       <c r="I8" s="46"/>
       <c r="J8" s="46"/>
       <c r="K8" s="46"/>
-      <c r="L8" s="164"/>
+      <c r="L8" s="156"/>
     </row>
     <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="153"/>
       <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="154" t="s">
+      <c r="D9" s="155" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -2651,8 +2651,8 @@
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
-      <c r="D10" s="155"/>
+      <c r="A10" s="153"/>
+      <c r="D10" s="153"/>
       <c r="E10" t="s">
         <v>2</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="H10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="159" t="s">
+      <c r="L10" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M10" s="57" t="s">
@@ -2673,18 +2673,18 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="156"/>
-      <c r="D11" s="156"/>
+      <c r="A11" s="154"/>
+      <c r="D11" s="154"/>
       <c r="E11" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="164"/>
+      <c r="L11" s="156"/>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157" t="s">
+      <c r="A12" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -2693,7 +2693,7 @@
       <c r="C12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="157" t="s">
+      <c r="D12" s="152" t="s">
         <v>81</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -2711,7 +2711,7 @@
       <c r="I12" s="36"/>
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
-      <c r="L12" s="166" t="s">
+      <c r="L12" s="157" t="s">
         <v>183</v>
       </c>
       <c r="M12" s="60" t="s">
@@ -2726,11 +2726,11 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
+      <c r="A13" s="153"/>
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="155"/>
+      <c r="D13" s="153"/>
       <c r="E13" t="s">
         <v>16</v>
       </c>
@@ -2743,16 +2743,16 @@
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
-      <c r="L13" s="167"/>
+      <c r="L13" s="158"/>
       <c r="M13" s="57" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="43"/>
       <c r="C14" s="43"/>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="155" t="s">
         <v>82</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -2770,7 +2770,7 @@
       <c r="I14" s="49"/>
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
-      <c r="L14" s="168" t="s">
+      <c r="L14" s="159" t="s">
         <v>180</v>
       </c>
       <c r="M14" s="59" t="s">
@@ -2785,8 +2785,8 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="156"/>
-      <c r="D15" s="156"/>
+      <c r="A15" s="154"/>
+      <c r="D15" s="154"/>
       <c r="E15" t="s">
         <v>16</v>
       </c>
@@ -2800,13 +2800,13 @@
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="169"/>
+      <c r="L15" s="160"/>
       <c r="M15" s="57" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -2844,7 +2844,7 @@
       <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
+      <c r="A17" s="153"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>21</v>
@@ -2858,7 +2858,7 @@
       <c r="H17" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="159" t="s">
+      <c r="L17" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M17" s="57" t="s">
@@ -2866,7 +2866,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
+      <c r="A18" s="153"/>
       <c r="D18" s="52"/>
       <c r="E18" s="53" t="s">
         <v>3</v>
@@ -2879,7 +2879,7 @@
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="164"/>
+      <c r="L18" s="156"/>
       <c r="M18" s="61"/>
       <c r="N18" s="56"/>
       <c r="O18" s="56"/>
@@ -2890,7 +2890,7 @@
       <c r="T18" s="56"/>
     </row>
     <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="I20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="163" t="s">
+      <c r="L20" s="166" t="s">
         <v>181</v>
       </c>
       <c r="M20" s="62" t="s">
@@ -2954,7 +2954,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
+      <c r="A21" s="153"/>
       <c r="D21" s="50"/>
       <c r="E21" t="s">
         <v>3</v>
@@ -2962,11 +2962,11 @@
       <c r="F21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="164"/>
+      <c r="L21" s="156"/>
       <c r="M21" s="62"/>
     </row>
     <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
+      <c r="A23" s="153"/>
       <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="J23" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="159" t="s">
+      <c r="L23" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M23" s="62" t="s">
@@ -3033,7 +3033,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="156"/>
+      <c r="A24" s="154"/>
       <c r="B24" s="3" t="s">
         <v>57</v>
       </c>
@@ -3044,10 +3044,10 @@
       <c r="F24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="160"/>
+      <c r="L24" s="161"/>
     </row>
     <row r="25" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -3085,7 +3085,7 @@
       <c r="T25" s="31"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="155"/>
+      <c r="A26" s="153"/>
       <c r="D26" s="50"/>
       <c r="E26" t="s">
         <v>45</v>
@@ -3096,7 +3096,7 @@
       <c r="G26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="163" t="s">
+      <c r="L26" s="166" t="s">
         <v>179</v>
       </c>
       <c r="M26" s="64" t="s">
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="153"/>
       <c r="D27" s="50"/>
       <c r="E27" t="s">
         <v>46</v>
@@ -3115,13 +3115,13 @@
       <c r="G27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L27" s="159"/>
+      <c r="L27" s="151"/>
       <c r="M27" s="57" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="155"/>
+      <c r="A28" s="153"/>
       <c r="D28" s="50"/>
       <c r="E28" t="s">
         <v>48</v>
@@ -3132,7 +3132,7 @@
       <c r="G28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="159" t="s">
+      <c r="L28" s="151" t="s">
         <v>174</v>
       </c>
       <c r="M28" s="57" t="s">
@@ -3140,7 +3140,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="156"/>
+      <c r="A29" s="154"/>
       <c r="D29" s="50"/>
       <c r="E29" t="s">
         <v>49</v>
@@ -3151,7 +3151,7 @@
       <c r="G29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L29" s="160"/>
+      <c r="L29" s="161"/>
       <c r="M29" s="57" t="s">
         <v>110</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D33" s="152" t="s">
+      <c r="D33" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E33" t="s">
@@ -3255,7 +3255,7 @@
       <c r="H33" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L33" s="159" t="s">
+      <c r="L33" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M33" s="57" t="s">
@@ -3263,17 +3263,17 @@
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="153"/>
+      <c r="D34" s="169"/>
       <c r="E34" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="159"/>
+      <c r="L34" s="151"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="152" t="s">
+      <c r="D35" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
@@ -3288,20 +3288,20 @@
       <c r="H35" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="159"/>
+      <c r="L35" s="151"/>
       <c r="M35" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="153"/>
+      <c r="D36" s="169"/>
       <c r="E36" t="s">
         <v>91</v>
       </c>
       <c r="F36" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="160"/>
+      <c r="L36" s="161"/>
     </row>
     <row r="37" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
@@ -3340,7 +3340,7 @@
       <c r="T37" s="31"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="152" t="s">
+      <c r="D38" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -3355,7 +3355,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="159" t="s">
+      <c r="L38" s="151" t="s">
         <v>173</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -3363,7 +3363,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="153"/>
+      <c r="D39" s="169"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -3371,10 +3371,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="159"/>
+      <c r="L39" s="151"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="152" t="s">
+      <c r="D40" s="164" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -3392,7 +3392,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="159" t="s">
+      <c r="L40" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -3400,14 +3400,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="153"/>
+      <c r="D41" s="169"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="160"/>
+      <c r="L41" s="161"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -3466,7 +3466,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="152" t="s">
+      <c r="D44" s="164" t="s">
         <v>73</v>
       </c>
       <c r="E44" t="s">
@@ -3484,7 +3484,7 @@
       <c r="I44" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L44" s="159" t="s">
+      <c r="L44" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M44" s="57" t="s">
@@ -3492,17 +3492,17 @@
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="153"/>
+      <c r="D45" s="169"/>
       <c r="E45" t="s">
         <v>91</v>
       </c>
       <c r="F45" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L45" s="159"/>
+      <c r="L45" s="151"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D46" s="152" t="s">
+      <c r="D46" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E46" t="s">
@@ -3514,7 +3514,7 @@
       <c r="G46" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="L46" s="163" t="s">
+      <c r="L46" s="166" t="s">
         <v>175</v>
       </c>
       <c r="M46" s="57" t="s">
@@ -3522,14 +3522,14 @@
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="172"/>
+      <c r="D47" s="165"/>
       <c r="E47" t="s">
         <v>127</v>
       </c>
       <c r="F47" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="L47" s="160"/>
+      <c r="L47" s="161"/>
       <c r="M47" s="57" t="s">
         <v>171</v>
       </c>
@@ -3593,7 +3593,7 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="152" t="s">
+      <c r="D50" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E50" s="42" t="s">
@@ -3605,7 +3605,7 @@
       <c r="G50" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="163" t="s">
+      <c r="L50" s="166" t="s">
         <v>175</v>
       </c>
       <c r="M50" s="57" t="s">
@@ -3613,14 +3613,14 @@
       </c>
     </row>
     <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="153"/>
+      <c r="D51" s="169"/>
       <c r="E51" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F51" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="160"/>
+      <c r="L51" s="161"/>
       <c r="M51" s="57" t="s">
         <v>152</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
-      <c r="L52" s="170" t="s">
+      <c r="L52" s="162" t="s">
         <v>182</v>
       </c>
       <c r="M52" s="60" t="s">
@@ -3672,13 +3672,13 @@
       <c r="G53" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L53" s="171"/>
+      <c r="L53" s="163"/>
       <c r="M53" s="57" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="152" t="s">
+      <c r="D54" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E54" t="s">
@@ -3693,7 +3693,7 @@
       <c r="H54" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="159" t="s">
+      <c r="L54" s="151" t="s">
         <v>167</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -3701,7 +3701,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="153"/>
+      <c r="D55" s="169"/>
       <c r="E55" t="s">
         <v>150</v>
       </c>
@@ -3714,7 +3714,7 @@
       <c r="H55" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="160"/>
+      <c r="L55" s="161"/>
       <c r="M55" s="57" t="s">
         <v>169</v>
       </c>
@@ -3744,7 +3744,7 @@
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
-      <c r="L56" s="165" t="s">
+      <c r="L56" s="150" t="s">
         <v>182</v>
       </c>
       <c r="M56" s="60" t="s">
@@ -3768,13 +3768,13 @@
       <c r="G57" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="159"/>
+      <c r="L57" s="151"/>
       <c r="M57" s="57" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="161" t="s">
+      <c r="D58" s="167" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -3786,7 +3786,7 @@
       <c r="G58" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="L58" s="159" t="s">
+      <c r="L58" s="151" t="s">
         <v>167</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -3794,7 +3794,7 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="162"/>
+      <c r="D59" s="168"/>
       <c r="E59" s="42" t="s">
         <v>164</v>
       </c>
@@ -3804,7 +3804,7 @@
       <c r="G59" s="136" t="s">
         <v>64</v>
       </c>
-      <c r="L59" s="160"/>
+      <c r="L59" s="161"/>
       <c r="M59" s="57" t="s">
         <v>166</v>
       </c>
@@ -3828,6 +3828,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="L33:L36"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L20:L21"/>
     <mergeCell ref="L56:L57"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="D14:D15"/>
@@ -3844,28 +3866,6 @@
     <mergeCell ref="L40:L41"/>
     <mergeCell ref="L44:L45"/>
     <mergeCell ref="L46:L47"/>
-    <mergeCell ref="L58:L59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="L33:L36"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D2:D8"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3917,7 +3917,7 @@
       <c r="R1" s="175"/>
     </row>
     <row r="2" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -3972,7 +3972,7 @@
       <c r="AA2" s="31"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="155"/>
+      <c r="A3" s="153"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
+      <c r="A4" s="153"/>
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -4016,7 +4016,7 @@
       <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="AA5" s="10"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="153"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -4094,13 +4094,13 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="156"/>
+      <c r="A7" s="154"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4150,7 +4150,7 @@
       <c r="AA8" s="31"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="156"/>
+      <c r="A9" s="154"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -4177,7 +4177,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="157" t="s">
+      <c r="A10" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -4221,7 +4221,7 @@
       <c r="AA10" s="31"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
+      <c r="A11" s="153"/>
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4239,7 +4239,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
+      <c r="A12" s="153"/>
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -4251,13 +4251,13 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
+      <c r="A13" s="153"/>
       <c r="T13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -4328,7 +4328,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
+      <c r="A16" s="153"/>
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -4337,7 +4337,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
+      <c r="A17" s="153"/>
       <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4381,7 +4381,7 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
+      <c r="A18" s="153"/>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
@@ -4408,7 +4408,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="156"/>
+      <c r="A19" s="154"/>
       <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
@@ -4417,7 +4417,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="157" t="s">
+      <c r="A20" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4459,7 +4459,7 @@
       <c r="AA20" s="31"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
+      <c r="A21" s="153"/>
       <c r="D21" t="s">
         <v>4</v>
       </c>
@@ -4474,7 +4474,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
+      <c r="A22" s="153"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
@@ -4489,7 +4489,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
+      <c r="A23" s="153"/>
       <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
@@ -4526,7 +4526,7 @@
       <c r="AA23" s="10"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="153"/>
       <c r="D24" t="s">
         <v>45</v>
       </c>
@@ -4541,7 +4541,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
+      <c r="A25" s="153"/>
       <c r="D25" t="s">
         <v>46</v>
       </c>
@@ -4556,7 +4556,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="155"/>
+      <c r="A26" s="153"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="156"/>
+      <c r="A27" s="154"/>
       <c r="D27" t="s">
         <v>49</v>
       </c>
@@ -4708,14 +4708,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="150" t="s">
+      <c r="F1" s="170" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="171"/>
+      <c r="K1" s="171"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -4724,7 +4724,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="152" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -4733,7 +4733,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="157" t="s">
+      <c r="D2" s="152" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -4766,8 +4766,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="155"/>
-      <c r="D3" s="155"/>
+      <c r="A3" s="153"/>
+      <c r="D3" s="153"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -4780,7 +4780,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="159" t="s">
+      <c r="L3" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -4788,8 +4788,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
-      <c r="D4" s="158"/>
+      <c r="A4" s="153"/>
+      <c r="D4" s="172"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -4800,20 +4800,20 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="164"/>
+      <c r="L4" s="156"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="154" t="s">
+      <c r="D5" s="155" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4846,8 +4846,8 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
-      <c r="D6" s="155"/>
+      <c r="A6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="E6" t="s">
         <v>2</v>
       </c>
@@ -4860,7 +4860,7 @@
       <c r="H6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="159" t="s">
+      <c r="L6" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="57" t="s">
@@ -4868,18 +4868,18 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="156"/>
-      <c r="D7" s="156"/>
+      <c r="A7" s="154"/>
+      <c r="D7" s="154"/>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="164"/>
+      <c r="L7" s="156"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="152" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4888,7 +4888,7 @@
       <c r="C8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="157" t="s">
+      <c r="D8" s="152" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4919,11 +4919,11 @@
       <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="153"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="155"/>
+      <c r="D9" s="153"/>
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -4942,10 +4942,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
-      <c r="D10" s="154" t="s">
+      <c r="D10" s="155" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -4974,8 +4974,8 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="156"/>
-      <c r="D11" s="156"/>
+      <c r="A11" s="154"/>
+      <c r="D11" s="154"/>
       <c r="E11" t="s">
         <v>16</v>
       </c>
@@ -4995,7 +4995,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157" t="s">
+      <c r="A12" s="152" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -5033,7 +5033,7 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
+      <c r="A13" s="153"/>
       <c r="D13" s="50"/>
       <c r="E13" t="s">
         <v>21</v>
@@ -5053,7 +5053,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
+      <c r="A14" s="153"/>
       <c r="D14" s="52"/>
       <c r="E14" s="53" t="s">
         <v>3</v>
@@ -5077,7 +5077,7 @@
       <c r="T14" s="56"/>
     </row>
     <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
@@ -5139,7 +5139,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
+      <c r="A17" s="153"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>3</v>
@@ -5151,7 +5151,7 @@
       <c r="M17" s="62"/>
     </row>
     <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
+      <c r="A18" s="153"/>
       <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
@@ -5216,7 +5216,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="156"/>
+      <c r="A20" s="154"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -5230,7 +5230,7 @@
       <c r="L20" s="116"/>
     </row>
     <row r="21" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="152" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -5266,7 +5266,7 @@
       <c r="T21" s="31"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
+      <c r="A22" s="153"/>
       <c r="D22" s="50"/>
       <c r="E22" t="s">
         <v>45</v>
@@ -5283,7 +5283,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
+      <c r="A23" s="153"/>
       <c r="D23" s="50"/>
       <c r="E23" t="s">
         <v>46</v>
@@ -5300,7 +5300,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="153"/>
       <c r="D24" s="50"/>
       <c r="E24" t="s">
         <v>48</v>
@@ -5317,7 +5317,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="156"/>
+      <c r="A25" s="154"/>
       <c r="D25" s="50"/>
       <c r="E25" t="s">
         <v>49</v>
@@ -5417,7 +5417,7 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="152" t="s">
+      <c r="D29" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
@@ -5432,7 +5432,7 @@
       <c r="H29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="159" t="s">
+      <c r="L29" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M29" s="57" t="s">
@@ -5440,7 +5440,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="153"/>
+      <c r="D30" s="169"/>
       <c r="E30" t="s">
         <v>4</v>
       </c>
@@ -5450,10 +5450,10 @@
       <c r="G30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="159"/>
+      <c r="L30" s="151"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="152" t="s">
+      <c r="D31" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
@@ -5468,13 +5468,13 @@
       <c r="H31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="159"/>
+      <c r="L31" s="151"/>
       <c r="M31" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="153"/>
+      <c r="D32" s="169"/>
       <c r="E32" t="s">
         <v>49</v>
       </c>
@@ -5484,7 +5484,7 @@
       <c r="G32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L32" s="160"/>
+      <c r="L32" s="161"/>
     </row>
     <row r="33" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
@@ -5542,7 +5542,7 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="152" t="s">
+      <c r="D35" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -5557,7 +5557,7 @@
       <c r="H35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="159" t="s">
+      <c r="L35" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="57" t="s">
@@ -5565,7 +5565,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="176"/>
+      <c r="D36" s="178"/>
       <c r="E36" s="43" t="s">
         <v>3</v>
       </c>
@@ -5603,7 +5603,7 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="152" t="s">
+      <c r="D38" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -5618,7 +5618,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="159" t="s">
+      <c r="L38" s="151" t="s">
         <v>131</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -5626,7 +5626,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="153"/>
+      <c r="D39" s="169"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -5634,10 +5634,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="159"/>
+      <c r="L39" s="151"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="152" t="s">
+      <c r="D40" s="164" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -5655,7 +5655,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="159" t="s">
+      <c r="L40" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -5663,14 +5663,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="153"/>
+      <c r="D41" s="169"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="160"/>
+      <c r="L41" s="161"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -5712,7 +5712,7 @@
       <c r="T42" s="31"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="152" t="s">
+      <c r="D43" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
@@ -5727,7 +5727,7 @@
       <c r="H43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="159" t="s">
+      <c r="L43" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -5735,7 +5735,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="153"/>
+      <c r="D44" s="169"/>
       <c r="E44" t="s">
         <v>124</v>
       </c>
@@ -5745,13 +5745,13 @@
       <c r="G44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="159"/>
+      <c r="L44" s="151"/>
       <c r="M44" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="152" t="s">
+      <c r="D45" s="164" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -5769,7 +5769,7 @@
       <c r="I45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="159" t="s">
+      <c r="L45" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M45" s="57" t="s">
@@ -5777,7 +5777,7 @@
       </c>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="176"/>
+      <c r="D46" s="178"/>
       <c r="E46" t="s">
         <v>91</v>
       </c>
@@ -5833,7 +5833,7 @@
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="152" t="s">
+      <c r="D49" s="164" t="s">
         <v>73</v>
       </c>
       <c r="E49" t="s">
@@ -5851,7 +5851,7 @@
       <c r="I49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="159" t="s">
+      <c r="L49" s="151" t="s">
         <v>103</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -5859,17 +5859,17 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="153"/>
+      <c r="D50" s="169"/>
       <c r="E50" t="s">
         <v>91</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="159"/>
+      <c r="L50" s="151"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D51" s="152" t="s">
+      <c r="D51" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E51" t="s">
@@ -5881,7 +5881,7 @@
       <c r="G51" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L51" s="163" t="s">
+      <c r="L51" s="166" t="s">
         <v>158</v>
       </c>
       <c r="M51" s="57" t="s">
@@ -5889,14 +5889,14 @@
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="172"/>
+      <c r="D52" s="165"/>
       <c r="E52" t="s">
         <v>127</v>
       </c>
       <c r="F52" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="160"/>
+      <c r="L52" s="161"/>
       <c r="M52" s="57" t="s">
         <v>154</v>
       </c>
@@ -5943,7 +5943,7 @@
       <c r="T53" s="31"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="152" t="s">
+      <c r="D54" s="164" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="42" t="s">
@@ -5958,7 +5958,7 @@
       <c r="H54" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="159" t="s">
+      <c r="L54" s="151" t="s">
         <v>102</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -5966,7 +5966,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="178"/>
+      <c r="D55" s="176"/>
       <c r="E55" s="42" t="s">
         <v>4</v>
       </c>
@@ -6031,7 +6031,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="152" t="s">
+      <c r="D58" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -6043,7 +6043,7 @@
       <c r="G58" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="163" t="s">
+      <c r="L58" s="166" t="s">
         <v>158</v>
       </c>
       <c r="M58" s="57" t="s">
@@ -6051,14 +6051,14 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="153"/>
+      <c r="D59" s="169"/>
       <c r="E59" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F59" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="160"/>
+      <c r="L59" s="161"/>
       <c r="M59" s="57" t="s">
         <v>152</v>
       </c>
@@ -6182,7 +6182,7 @@
       </c>
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D65" s="152" t="s">
+      <c r="D65" s="164" t="s">
         <v>74</v>
       </c>
       <c r="E65" t="s">
@@ -6197,7 +6197,7 @@
       <c r="H65" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L65" s="159" t="s">
+      <c r="L65" s="151" t="s">
         <v>162</v>
       </c>
       <c r="M65" s="57" t="s">
@@ -6205,7 +6205,7 @@
       </c>
     </row>
     <row r="66" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="153"/>
+      <c r="D66" s="169"/>
       <c r="E66" t="s">
         <v>150</v>
       </c>
@@ -6218,7 +6218,7 @@
       <c r="H66" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L66" s="160"/>
+      <c r="L66" s="161"/>
       <c r="M66" s="57" t="s">
         <v>147</v>
       </c>
@@ -6242,6 +6242,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="L45:L46"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D65:D66"/>
@@ -6252,30 +6276,6 @@
     <mergeCell ref="L51:L52"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L54:L55"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
add test to check item_ops and update doc
</commit_message>
<xml_diff>
--- a/doc/ops.xlsx
+++ b/doc/ops.xlsx
@@ -12,7 +12,7 @@
     <sheet name="stack op 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'stack op'!$A$31:$M$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'stack op'!$A$36:$T$64</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'stack op 2'!$A$27:$M$66</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="232">
   <si>
     <t>A → α β+ γ</t>
   </si>
@@ -953,40 +953,6 @@
 |child_fact(A1)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">L: exit_A2 → iter_A(ctx={β}) </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R: collects all βs into an array</t>
-    </r>
-  </si>
-  <si>
-    <t>(&amp; left factorization)</t>
-  </si>
-  <si>
-    <t>child_+*(A)
-|parent_fact</t>
-  </si>
-  <si>
     <t>child_fact(A)
 |parent_fact</t>
   </si>
@@ -1000,25 +966,6 @@
   <si>
     <t>L|r_rec
 |parent_fact</t>
-  </si>
-  <si>
-    <t>L|r_rec</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">exit_A → exit_A(ctx={α})  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(could be optimized by using opcode similar to L-form + priority(0), ...)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1046,6 +993,187 @@
       </rPr>
       <t xml:space="preserve"> R: exit_A(ctx={[α], β})</t>
     </r>
+  </si>
+  <si>
+    <t>A → α β</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>A → α B β</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>push</t>
+  </si>
+  <si>
+    <t>γ</t>
+  </si>
+  <si>
+    <t>[A1]</t>
+  </si>
+  <si>
+    <t>item_ops (pop right 1st)</t>
+  </si>
+  <si>
+    <t>(and left factor.)</t>
+  </si>
+  <si>
+    <t>opcodes (pop right 1st)</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={α, A1, γ})</t>
+  </si>
+  <si>
+    <t>parent_+*|L</t>
+  </si>
+  <si>
+    <t>parent_+*|+</t>
+  </si>
+  <si>
+    <t>child_+*(A)|+|L
+|parent_fact</t>
+  </si>
+  <si>
+    <t>child_+*(A)|+
+|parent_fact</t>
+  </si>
+  <si>
+    <t>exit(0)</t>
+  </si>
+  <si>
+    <t>exit(2)</t>
+  </si>
+  <si>
+    <t>exit(3)</t>
+  </si>
+  <si>
+    <t>#f</t>
+  </si>
+  <si>
+    <t>call to internal wrapper → actions / call to public listener methods</t>
+  </si>
+  <si>
+    <t>exit_AIter1 → exit_AIter1(ctx={A1, β, last=false})</t>
+  </si>
+  <si>
+    <t>exit_AIter1 → exit_AIter1(ctx={A1, β, last=true})</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={α, [A1], γ})</t>
+  </si>
+  <si>
+    <t>init_A1 → push empty [A1]</t>
+  </si>
+  <si>
+    <t>exit_A1 → [A1].push(β)</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={α, γ}) &amp; push</t>
+  </si>
+  <si>
+    <t>init_A1 → init_AIter1() &amp; ...</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={α, B, β}) &amp; push</t>
+  </si>
+  <si>
+    <t>exit_AIter1 → exit_AIter1(ctx={A1})</t>
+  </si>
+  <si>
+    <t>init_A1 → init_AIter1() / exit_AIter1 → exit_AIter1(ctx={A1, β})</t>
+  </si>
+  <si>
+    <t>init_A1 → push empty [A1] / exit_A1 → [A1].push(β)</t>
+  </si>
+  <si>
+    <t>i:[A1]</t>
+  </si>
+  <si>
+    <t>i:A1</t>
+  </si>
+  <si>
+    <t>e:[A1]</t>
+  </si>
+  <si>
+    <t>e:b</t>
+  </si>
+  <si>
+    <t>e:A1</t>
+  </si>
+  <si>
+    <t>exit(1)</t>
+  </si>
+  <si>
+    <t>r_rec|L</t>
+  </si>
+  <si>
+    <t>e:A</t>
+  </si>
+  <si>
+    <t>e:α</t>
+  </si>
+  <si>
+    <t>exit_A → exit_A(ctx={A, α})</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">exit_A → iter_A(ctx={A, β})   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(last called)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">exit_A → exit_A(ctx={ β})     </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(first called)</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: "●A1" calls loop_A1, whereas "A1" calls enter_A1; i: and e: are for "init-"/"exit-only" when both have an action</t>
+  </si>
+  <si>
+    <t>init_A → init_A() / exit_A → iter_A(ctx={A, α})</t>
+  </si>
+  <si>
+    <t>inter_A → exit_A(ctx={β})</t>
+  </si>
+  <si>
+    <t>exit_A1 → exit_A(ctx={A})</t>
+  </si>
+  <si>
+    <t>ζ</t>
+  </si>
+  <si>
+    <t>δ</t>
+  </si>
+  <si>
+    <t>exit(4)</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1194,8 +1322,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1584,11 +1718,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1999,27 +2172,63 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2032,59 +2241,237 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2390,10 +2777,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,1470 +2790,2166 @@
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="19" customWidth="1"/>
-    <col min="7" max="11" width="7.5703125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="87.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="4" customWidth="1"/>
-    <col min="15" max="20" width="9.140625" style="4"/>
+    <col min="5" max="5" width="3.7109375" style="224" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="19" customWidth="1"/>
+    <col min="8" max="12" width="7.5703125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="75" customWidth="1"/>
+    <col min="14" max="18" width="5.7109375" style="193" customWidth="1"/>
+    <col min="19" max="19" width="9" style="192" customWidth="1"/>
+    <col min="20" max="20" width="87.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="4" customWidth="1"/>
+    <col min="22" max="27" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="224" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="170" t="s">
-        <v>134</v>
-      </c>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
-      <c r="L1" s="116" t="s">
+      <c r="G1" s="182" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="183"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="183"/>
+      <c r="K1" s="183"/>
+      <c r="L1" s="183"/>
+      <c r="M1" s="116" t="s">
         <v>159</v>
       </c>
-      <c r="M1" s="89" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="152" t="s">
+      <c r="N1" s="217" t="s">
+        <v>189</v>
+      </c>
+      <c r="O1" s="218"/>
+      <c r="P1" s="218"/>
+      <c r="Q1" s="218"/>
+      <c r="R1" s="219"/>
+      <c r="S1" s="192" t="s">
+        <v>186</v>
+      </c>
+      <c r="T1" s="89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="186" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="184"/>
+      <c r="B2" s="185" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="186" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="184"/>
+      <c r="E2" s="225">
+        <v>0</v>
+      </c>
+      <c r="F2" s="186" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="190" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" s="191" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="191" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="187">
+        <v>0</v>
+      </c>
+      <c r="N2" s="190" t="s">
+        <v>184</v>
+      </c>
+      <c r="O2" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="191" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q2" s="191"/>
+      <c r="R2" s="191"/>
+      <c r="S2" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="T2" s="188" t="s">
+        <v>209</v>
+      </c>
+      <c r="U2" s="189"/>
+      <c r="V2" s="189"/>
+      <c r="W2" s="189"/>
+      <c r="X2" s="189"/>
+      <c r="Y2" s="189"/>
+      <c r="Z2" s="189"/>
+      <c r="AA2" s="189"/>
+    </row>
+    <row r="3" spans="1:27" s="143" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="160" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="220" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C3" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="152" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="D3" s="160" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="226">
+        <v>0</v>
+      </c>
+      <c r="F3" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="G3" s="144" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I3" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="J3" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" t="s">
+      <c r="K3" s="145"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="146" t="s">
+        <v>194</v>
+      </c>
+      <c r="N3" s="194" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="195" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="195" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q3" s="195"/>
+      <c r="R3" s="195"/>
+      <c r="S3" s="194" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="147" t="s">
+        <v>207</v>
+      </c>
+      <c r="U3" s="148"/>
+      <c r="V3" s="148"/>
+      <c r="W3" s="148"/>
+      <c r="X3" s="148"/>
+      <c r="Y3" s="148"/>
+      <c r="Z3" s="148"/>
+      <c r="AA3" s="148"/>
+    </row>
+    <row r="4" spans="1:27" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="158"/>
+      <c r="B4" s="221" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="158"/>
+      <c r="E4" s="227">
+        <v>1</v>
+      </c>
+      <c r="F4" s="138" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="141" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="142" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="130" t="s">
+        <v>195</v>
+      </c>
+      <c r="N4" s="196"/>
+      <c r="O4" s="197"/>
+      <c r="P4" s="197"/>
+      <c r="Q4" s="197"/>
+      <c r="R4" s="197"/>
+      <c r="S4" s="196" t="s">
+        <v>214</v>
+      </c>
+      <c r="T4" s="140" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="227">
         <v>2</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F5" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="46" t="s">
+      <c r="H5" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="162" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="S5" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="227">
+        <v>3</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="167"/>
+      <c r="N6" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="S6" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="57" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="158"/>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="228">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="222" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="223" t="s">
+        <v>194</v>
+      </c>
+      <c r="N7" s="213" t="s">
+        <v>184</v>
+      </c>
+      <c r="O7" s="214" t="s">
+        <v>188</v>
+      </c>
+      <c r="P7" s="214" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q7" s="214"/>
+      <c r="R7" s="214"/>
+      <c r="S7" s="213" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+    </row>
+    <row r="8" spans="1:27" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="158"/>
+      <c r="B8" s="221" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="158"/>
+      <c r="E8" s="227">
+        <v>1</v>
+      </c>
+      <c r="F8" s="138" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="141" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="151" t="s">
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="150" t="s">
+        <v>196</v>
+      </c>
+      <c r="N8" s="196"/>
+      <c r="O8" s="197"/>
+      <c r="P8" s="197"/>
+      <c r="Q8" s="197"/>
+      <c r="R8" s="197"/>
+      <c r="S8" s="196" t="s">
+        <v>213</v>
+      </c>
+      <c r="T8" s="140" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="158"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="227">
+        <v>2</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="162" t="s">
+        <v>174</v>
+      </c>
+      <c r="N9" s="192" t="s">
+        <v>188</v>
+      </c>
+      <c r="O9" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="S9" s="192" t="s">
+        <v>188</v>
+      </c>
+      <c r="T9" s="57" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="158"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="227">
+        <v>3</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="167"/>
+      <c r="N10" s="192" t="s">
+        <v>188</v>
+      </c>
+      <c r="O10" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="S10" s="192" t="s">
+        <v>188</v>
+      </c>
+      <c r="T10" s="57" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="158"/>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="157" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="228">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" s="152" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="152" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="152"/>
+      <c r="L11" s="152"/>
+      <c r="M11" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="N11" s="213" t="s">
+        <v>184</v>
+      </c>
+      <c r="O11" s="214" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="214" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q11" s="214"/>
+      <c r="R11" s="214"/>
+      <c r="S11" s="213" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="158"/>
+      <c r="D12" s="158"/>
+      <c r="E12" s="227">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="M3" s="57" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="46" t="s">
+      <c r="N12" s="192" t="s">
+        <v>217</v>
+      </c>
+      <c r="O12" s="193" t="s">
+        <v>216</v>
+      </c>
+      <c r="S12" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="158"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="227">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="M13" s="167"/>
+      <c r="N13" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="S13" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13" s="57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="158"/>
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="228">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="213" t="s">
+        <v>184</v>
+      </c>
+      <c r="O14" s="214" t="s">
+        <v>188</v>
+      </c>
+      <c r="P14" s="214" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q14" s="214"/>
+      <c r="R14" s="214"/>
+      <c r="S14" s="213" t="s">
+        <v>17</v>
+      </c>
+      <c r="T14" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="227">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="I15" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="L4" s="151"/>
-      <c r="M4" s="89" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="143" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="153"/>
-      <c r="B5" s="143" t="s">
+      <c r="M15" s="162" t="s">
+        <v>173</v>
+      </c>
+      <c r="N15" s="192" t="s">
+        <v>215</v>
+      </c>
+      <c r="O15" s="193" t="s">
+        <v>216</v>
+      </c>
+      <c r="S15" s="192" t="s">
+        <v>188</v>
+      </c>
+      <c r="T15" s="57" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="227">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="M16" s="167"/>
+      <c r="N16" s="192"/>
+    </row>
+    <row r="17" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="160" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="160" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="229">
+        <v>0</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="169" t="s">
+        <v>219</v>
+      </c>
+      <c r="N17" s="198" t="s">
+        <v>220</v>
+      </c>
+      <c r="O17" s="199" t="s">
+        <v>221</v>
+      </c>
+      <c r="P17" s="199"/>
+      <c r="Q17" s="199"/>
+      <c r="R17" s="199"/>
+      <c r="S17" s="198" t="s">
+        <v>17</v>
+      </c>
+      <c r="T17" s="232" t="s">
+        <v>226</v>
+      </c>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="158"/>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="158"/>
+      <c r="E18" s="227">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="H18" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="170"/>
+      <c r="N18" s="200" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="139" t="s">
+        <v>185</v>
+      </c>
+      <c r="P18" s="139"/>
+      <c r="Q18" s="139"/>
+      <c r="R18" s="139"/>
+      <c r="S18" s="200"/>
+      <c r="T18" s="57" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="158"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="228">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="171" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="153"/>
-      <c r="E5" s="143" t="s">
+      <c r="N19" s="201" t="s">
+        <v>184</v>
+      </c>
+      <c r="O19" s="202" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19" s="202"/>
+      <c r="Q19" s="202"/>
+      <c r="R19" s="202"/>
+      <c r="S19" s="201" t="s">
+        <v>17</v>
+      </c>
+      <c r="T19" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+    </row>
+    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="227">
         <v>1</v>
       </c>
-      <c r="F5" s="144" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="145" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="145" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="145" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="145"/>
-      <c r="K5" s="145"/>
-      <c r="L5" s="146"/>
-      <c r="M5" s="147" t="s">
-        <v>118</v>
-      </c>
-      <c r="N5" s="148"/>
-      <c r="O5" s="148"/>
-      <c r="P5" s="148"/>
-      <c r="Q5" s="148"/>
-      <c r="R5" s="148"/>
-      <c r="S5" s="148"/>
-      <c r="T5" s="148"/>
-    </row>
-    <row r="6" spans="1:20" s="137" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="153"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="138" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="141" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="142" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="130" t="s">
-        <v>178</v>
-      </c>
-      <c r="M6" s="140"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="153"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="151" t="s">
-        <v>174</v>
-      </c>
-      <c r="M7" s="57" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="153"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="156"/>
-    </row>
-    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="153"/>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="155" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="118"/>
-      <c r="M9" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="153"/>
-      <c r="D10" s="153"/>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="151" t="s">
-        <v>173</v>
-      </c>
-      <c r="M10" s="57" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="156"/>
-    </row>
-    <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="152" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="157" t="s">
-        <v>183</v>
-      </c>
-      <c r="M12" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="153"/>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="153"/>
-      <c r="E13" t="s">
+      <c r="F20" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="158"/>
-      <c r="M13" s="57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="155" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="159" t="s">
-        <v>180</v>
-      </c>
-      <c r="M14" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-    </row>
-    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="46"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="160"/>
-      <c r="M15" s="57" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="152" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="153"/>
-      <c r="D17" s="50"/>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="151" t="s">
-        <v>103</v>
-      </c>
-      <c r="M17" s="57" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="153"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="156"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-    </row>
-    <row r="19" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="153"/>
-      <c r="B19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="118"/>
-      <c r="M19" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="153"/>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
+      <c r="G20" s="47" t="s">
+        <v>218</v>
       </c>
       <c r="H20" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="46" t="s">
+      <c r="I20" s="46"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="172"/>
+      <c r="N20" s="200" t="s">
+        <v>185</v>
+      </c>
+      <c r="O20" s="139"/>
+      <c r="P20" s="139"/>
+      <c r="Q20" s="139"/>
+      <c r="R20" s="139"/>
+      <c r="S20" s="200" t="s">
+        <v>17</v>
+      </c>
+      <c r="T20" s="57" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="160" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="229">
+        <v>0</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="I21" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="211" t="s">
+        <v>185</v>
+      </c>
+      <c r="O21" s="212"/>
+      <c r="P21" s="212"/>
+      <c r="Q21" s="212"/>
+      <c r="R21" s="212"/>
+      <c r="S21" s="211" t="s">
+        <v>17</v>
+      </c>
+      <c r="T21" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="158"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="224">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="I22" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="166" t="s">
-        <v>181</v>
-      </c>
-      <c r="M20" s="62" t="s">
+      <c r="M22" s="162" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="193" t="s">
+        <v>184</v>
+      </c>
+      <c r="S22" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="T22" s="57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="158"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="230">
+        <v>2</v>
+      </c>
+      <c r="F23" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="167"/>
+      <c r="N23" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="204"/>
+      <c r="P23" s="204"/>
+      <c r="Q23" s="204"/>
+      <c r="R23" s="204"/>
+      <c r="S23" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="T23" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="56"/>
+      <c r="AA23" s="56"/>
+    </row>
+    <row r="24" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="158"/>
+      <c r="B24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="51"/>
+      <c r="E24" s="228"/>
+      <c r="F24" s="233" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="234" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="235" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="236" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="235"/>
+      <c r="K24" s="235"/>
+      <c r="L24" s="235"/>
+      <c r="M24" s="237"/>
+      <c r="N24" s="238"/>
+      <c r="O24" s="239"/>
+      <c r="P24" s="239"/>
+      <c r="Q24" s="239"/>
+      <c r="R24" s="239"/>
+      <c r="S24" s="238"/>
+      <c r="T24" s="240" t="s">
+        <v>115</v>
+      </c>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="158"/>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="F25" s="241" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="242" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="243" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="244" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="244" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="245"/>
+      <c r="L25" s="245"/>
+      <c r="M25" s="246" t="s">
+        <v>178</v>
+      </c>
+      <c r="N25" s="247"/>
+      <c r="O25" s="248"/>
+      <c r="P25" s="248"/>
+      <c r="Q25" s="248"/>
+      <c r="R25" s="248"/>
+      <c r="S25" s="247"/>
+      <c r="T25" s="249" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="153"/>
-      <c r="D21" s="50"/>
-      <c r="E21" t="s">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="158"/>
+      <c r="D26" s="50"/>
+      <c r="F26" s="241" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="G26" s="250" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="156"/>
-      <c r="M21" s="62"/>
-    </row>
-    <row r="22" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="153"/>
-      <c r="B22" s="7" t="s">
+      <c r="H26" s="245"/>
+      <c r="I26" s="245"/>
+      <c r="J26" s="245"/>
+      <c r="K26" s="245"/>
+      <c r="L26" s="245"/>
+      <c r="M26" s="251"/>
+      <c r="N26" s="215"/>
+      <c r="O26" s="216"/>
+      <c r="P26" s="216"/>
+      <c r="Q26" s="216"/>
+      <c r="R26" s="216"/>
+      <c r="S26" s="215"/>
+      <c r="T26" s="249"/>
+    </row>
+    <row r="27" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="158"/>
+      <c r="B27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="7" t="s">
+      <c r="D27" s="51"/>
+      <c r="E27" s="228"/>
+      <c r="F27" s="233" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="G27" s="234" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H27" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="I27" s="235" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="59" t="s">
+      <c r="J27" s="235"/>
+      <c r="K27" s="235"/>
+      <c r="L27" s="235"/>
+      <c r="M27" s="237"/>
+      <c r="N27" s="238"/>
+      <c r="O27" s="239"/>
+      <c r="P27" s="239"/>
+      <c r="Q27" s="239"/>
+      <c r="R27" s="239"/>
+      <c r="S27" s="238"/>
+      <c r="T27" s="240" t="s">
         <v>104</v>
       </c>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="153"/>
-      <c r="B23" s="3" t="s">
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="158"/>
+      <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" t="s">
+      <c r="D28" s="50"/>
+      <c r="F28" s="241" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="G28" s="242" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="H28" s="243" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="46" t="s">
+      <c r="I28" s="244" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="J28" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="46" t="s">
+      <c r="K28" s="244" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="151" t="s">
+      <c r="L28" s="245"/>
+      <c r="M28" s="252" t="s">
         <v>103</v>
       </c>
-      <c r="M23" s="62" t="s">
+      <c r="N28" s="215"/>
+      <c r="O28" s="216"/>
+      <c r="P28" s="216"/>
+      <c r="Q28" s="216"/>
+      <c r="R28" s="216"/>
+      <c r="S28" s="215"/>
+      <c r="T28" s="249" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="154"/>
-      <c r="B24" s="3" t="s">
+    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="159"/>
+      <c r="B29" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" t="s">
+      <c r="D29" s="50"/>
+      <c r="F29" s="241" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="G29" s="250" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="161"/>
-    </row>
-    <row r="25" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="152" t="s">
+      <c r="H29" s="245"/>
+      <c r="I29" s="245"/>
+      <c r="J29" s="245"/>
+      <c r="K29" s="245"/>
+      <c r="L29" s="245"/>
+      <c r="M29" s="253"/>
+      <c r="N29" s="215"/>
+      <c r="O29" s="216"/>
+      <c r="P29" s="216"/>
+      <c r="Q29" s="216"/>
+      <c r="R29" s="216"/>
+      <c r="S29" s="215"/>
+      <c r="T29" s="254"/>
+    </row>
+    <row r="30" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="160" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B30" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C30" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="25" t="s">
+      <c r="D30" s="48"/>
+      <c r="E30" s="229">
+        <v>0</v>
+      </c>
+      <c r="F30" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="G30" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="H30" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="117" t="s">
-        <v>160</v>
-      </c>
-      <c r="M25" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="153"/>
-      <c r="D26" s="50"/>
-      <c r="E26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="166" t="s">
-        <v>179</v>
-      </c>
-      <c r="M26" s="64" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="153"/>
-      <c r="D27" s="50"/>
-      <c r="E27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="151"/>
-      <c r="M27" s="57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="153"/>
-      <c r="D28" s="50"/>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="151" t="s">
-        <v>174</v>
-      </c>
-      <c r="M28" s="57" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="154"/>
-      <c r="D29" s="50"/>
-      <c r="E29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="161"/>
-      <c r="M29" s="57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="86" t="s">
-        <v>101</v>
-      </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-    </row>
-    <row r="31" spans="1:20" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="L30" s="27"/>
+      <c r="M30" s="117" t="s">
+        <v>160</v>
+      </c>
+      <c r="N30" s="211"/>
+      <c r="O30" s="212"/>
+      <c r="P30" s="212"/>
+      <c r="Q30" s="212"/>
+      <c r="R30" s="212"/>
+      <c r="S30" s="211"/>
+      <c r="T30" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="158"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="224">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="166" t="s">
+        <v>176</v>
+      </c>
+      <c r="N31" s="196"/>
+      <c r="O31" s="197"/>
+      <c r="P31" s="197"/>
+      <c r="Q31" s="197"/>
+      <c r="R31" s="197"/>
+      <c r="S31" s="196"/>
+      <c r="T31" s="64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="158"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="224">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="162"/>
+      <c r="N32" s="192" t="s">
+        <v>184</v>
+      </c>
+      <c r="O32" s="193" t="s">
+        <v>229</v>
+      </c>
+      <c r="S32" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="T32" s="57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="158"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="224">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="162" t="s">
+        <v>174</v>
+      </c>
+      <c r="N33" s="192" t="s">
+        <v>184</v>
+      </c>
+      <c r="O33" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="P33" s="193" t="s">
+        <v>187</v>
+      </c>
+      <c r="S33" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="T33" s="57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="159"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="224">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="163"/>
+      <c r="N34" s="192" t="s">
+        <v>184</v>
+      </c>
+      <c r="O34" s="193" t="s">
+        <v>185</v>
+      </c>
+      <c r="P34" s="193" t="s">
+        <v>230</v>
+      </c>
+      <c r="S34" s="192" t="s">
+        <v>17</v>
+      </c>
+      <c r="T34" s="57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="229"/>
+      <c r="G35" s="86" t="s">
+        <v>225</v>
+      </c>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="212"/>
+      <c r="O35" s="212"/>
+      <c r="P35" s="212"/>
+      <c r="Q35" s="212"/>
+      <c r="R35" s="212"/>
+      <c r="S35" s="211"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="31"/>
+      <c r="AA35" s="31"/>
+    </row>
+    <row r="36" spans="1:27" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="75" t="s">
+      <c r="E36" s="226"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="M31" s="75" t="s">
+      <c r="N36" s="193"/>
+      <c r="O36" s="193"/>
+      <c r="P36" s="193"/>
+      <c r="Q36" s="193"/>
+      <c r="R36" s="193"/>
+      <c r="S36" s="192"/>
+      <c r="T36" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="76"/>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="76"/>
-      <c r="S31" s="76"/>
-      <c r="T31" s="76"/>
-    </row>
-    <row r="32" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="76"/>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="76"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="76"/>
+    </row>
+    <row r="37" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C37" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E37" s="231"/>
+      <c r="F37" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="G37" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="H37" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="77" t="s">
+      <c r="I37" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="J37" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="77" t="s">
+      <c r="K37" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="K32" s="27" t="s">
+      <c r="L37" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="L32" s="117"/>
-      <c r="M32" s="60" t="s">
+      <c r="M37" s="117"/>
+      <c r="N37" s="211"/>
+      <c r="O37" s="212"/>
+      <c r="P37" s="212"/>
+      <c r="Q37" s="212"/>
+      <c r="R37" s="212"/>
+      <c r="S37" s="211"/>
+      <c r="T37" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="31"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D33" s="164" t="s">
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D38" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F38" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="66" t="s">
+      <c r="G38" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="67" t="s">
+      <c r="H38" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="I38" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L33" s="151" t="s">
+      <c r="M38" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="M33" s="57" t="s">
+      <c r="N38" s="192"/>
+      <c r="T38" s="57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="169"/>
-      <c r="E34" t="s">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D39" s="156"/>
+      <c r="F39" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="66" t="s">
+      <c r="G39" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="151"/>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="164" t="s">
+      <c r="M39" s="162"/>
+      <c r="N39" s="192"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D40" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F40" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="66" t="s">
+      <c r="G40" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="67" t="s">
+      <c r="H40" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="I40" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="151"/>
-      <c r="M35" s="57" t="s">
+      <c r="M40" s="162"/>
+      <c r="N40" s="192"/>
+      <c r="T40" s="57" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="169"/>
-      <c r="E36" t="s">
+    <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="156"/>
+      <c r="F41" t="s">
         <v>91</v>
       </c>
-      <c r="F36" s="66" t="s">
+      <c r="G41" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="161"/>
-    </row>
-    <row r="37" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="25" t="s">
+      <c r="M41" s="163"/>
+      <c r="N41" s="192"/>
+    </row>
+    <row r="42" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C42" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E42" s="229"/>
+      <c r="F42" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="131" t="s">
+      <c r="G42" s="131" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="132" t="s">
+      <c r="H42" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="133" t="s">
+      <c r="I42" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="117" t="s">
-        <v>161</v>
-      </c>
-      <c r="M37" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="31"/>
-      <c r="Q37" s="31"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="31"/>
-      <c r="T37" s="31"/>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="164" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="66" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L38" s="151" t="s">
-        <v>173</v>
-      </c>
-      <c r="M38" s="57" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="169"/>
-      <c r="E39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="65"/>
-      <c r="L39" s="151"/>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="164" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="L40" s="151" t="s">
-        <v>103</v>
-      </c>
-      <c r="M40" s="57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="169"/>
-      <c r="E41" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="83" t="s">
-        <v>69</v>
-      </c>
-      <c r="L41" s="161"/>
-    </row>
-    <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G42" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I42" s="27"/>
       <c r="J42" s="27"/>
       <c r="K42" s="27"/>
-      <c r="L42" s="117" t="s">
+      <c r="L42" s="27"/>
+      <c r="M42" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="M42" s="60" t="s">
+      <c r="N42" s="211"/>
+      <c r="O42" s="212"/>
+      <c r="P42" s="212"/>
+      <c r="Q42" s="212"/>
+      <c r="R42" s="212"/>
+      <c r="S42" s="211"/>
+      <c r="T42" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="31"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="92" t="s">
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="31"/>
+      <c r="Z42" s="31"/>
+      <c r="AA42" s="31"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D43" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="H43" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="M43" s="162" t="s">
+        <v>173</v>
+      </c>
+      <c r="N43" s="192"/>
+      <c r="T43" s="57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D44" s="156"/>
+      <c r="F44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="65"/>
+      <c r="M44" s="162"/>
+      <c r="N44" s="192"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D45" s="155" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="I45" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="162" t="s">
+        <v>103</v>
+      </c>
+      <c r="N45" s="192"/>
+      <c r="T45" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="156"/>
+      <c r="F46" t="s">
+        <v>91</v>
+      </c>
+      <c r="G46" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="M46" s="163"/>
+      <c r="N46" s="192"/>
+    </row>
+    <row r="47" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="229"/>
+      <c r="F47" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="117" t="s">
+        <v>161</v>
+      </c>
+      <c r="N47" s="211"/>
+      <c r="O47" s="212"/>
+      <c r="P47" s="212"/>
+      <c r="Q47" s="212"/>
+      <c r="R47" s="212"/>
+      <c r="S47" s="211"/>
+      <c r="T47" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31"/>
+      <c r="Y47" s="31"/>
+      <c r="Z47" s="31"/>
+      <c r="AA47" s="31"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D48" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
         <v>125</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="G48" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="G43" s="69" t="s">
+      <c r="H48" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="149" t="s">
+      <c r="M48" s="149" t="s">
         <v>160</v>
       </c>
-      <c r="M43" s="57" t="s">
+      <c r="N48" s="207"/>
+      <c r="O48" s="208"/>
+      <c r="P48" s="208"/>
+      <c r="Q48" s="208"/>
+      <c r="R48" s="208"/>
+      <c r="S48" s="207"/>
+      <c r="T48" s="57" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="164" t="s">
+    <row r="49" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D49" s="155" t="s">
         <v>73</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F49" t="s">
         <v>90</v>
       </c>
-      <c r="F44" s="19" t="s">
+      <c r="G49" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="H49" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="I49" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="J49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L44" s="151" t="s">
+      <c r="M49" s="162" t="s">
         <v>103</v>
       </c>
-      <c r="M44" s="57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="169"/>
-      <c r="E45" t="s">
+      <c r="N49" s="192"/>
+      <c r="T49" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D50" s="156"/>
+      <c r="F50" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="G50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L45" s="151"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D46" s="164" t="s">
+      <c r="M50" s="162"/>
+      <c r="N50" s="192"/>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D51" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F51" t="s">
         <v>126</v>
       </c>
-      <c r="F46" s="95" t="s">
+      <c r="G51" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="G46" s="93" t="s">
+      <c r="H51" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="L46" s="166" t="s">
+      <c r="M51" s="166" t="s">
         <v>175</v>
       </c>
-      <c r="M46" s="57" t="s">
+      <c r="N51" s="196"/>
+      <c r="O51" s="197"/>
+      <c r="P51" s="197"/>
+      <c r="Q51" s="197"/>
+      <c r="R51" s="197"/>
+      <c r="S51" s="196"/>
+      <c r="T51" s="57" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="165"/>
-      <c r="E47" t="s">
+    <row r="52" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="175"/>
+      <c r="F52" t="s">
         <v>127</v>
       </c>
-      <c r="F47" s="103" t="s">
+      <c r="G52" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="L47" s="161"/>
-      <c r="M47" s="57" t="s">
+      <c r="M52" s="163"/>
+      <c r="N52" s="192"/>
+      <c r="T52" s="57" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="25" t="s">
+    <row r="53" spans="2:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C53" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="74" t="s">
+      <c r="E53" s="231"/>
+      <c r="F53" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F48" s="26" t="s">
+      <c r="G53" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="27" t="s">
+      <c r="H53" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="27" t="s">
+      <c r="I53" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I48" s="27" t="s">
+      <c r="J53" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="117" t="s">
+      <c r="K53" s="27"/>
+      <c r="L53" s="27"/>
+      <c r="M53" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="M48" s="60" t="s">
+      <c r="N53" s="211"/>
+      <c r="O53" s="212"/>
+      <c r="P53" s="212"/>
+      <c r="Q53" s="212"/>
+      <c r="R53" s="212"/>
+      <c r="S53" s="211"/>
+      <c r="T53" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="N48" s="31"/>
-      <c r="O48" s="31"/>
-      <c r="P48" s="31"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="31"/>
-      <c r="S48" s="31"/>
-      <c r="T48" s="31"/>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="92" t="s">
+      <c r="U53" s="31"/>
+      <c r="V53" s="31"/>
+      <c r="W53" s="31"/>
+      <c r="X53" s="31"/>
+      <c r="Y53" s="31"/>
+      <c r="Z53" s="31"/>
+      <c r="AA53" s="31"/>
+    </row>
+    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D54" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E54" s="227"/>
+      <c r="F54" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="G54" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G49" s="98" t="s">
+      <c r="H54" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L49" s="149" t="s">
+      <c r="M54" s="149" t="s">
         <v>160</v>
       </c>
-      <c r="M49" s="57" t="s">
+      <c r="N54" s="207"/>
+      <c r="O54" s="208"/>
+      <c r="P54" s="208"/>
+      <c r="Q54" s="208"/>
+      <c r="R54" s="208"/>
+      <c r="S54" s="207"/>
+      <c r="T54" s="57" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="164" t="s">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D55" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E55" s="227"/>
+      <c r="F55" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="F50" s="95" t="s">
+      <c r="G55" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="G50" s="93" t="s">
+      <c r="H55" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="166" t="s">
+      <c r="M55" s="166" t="s">
         <v>175</v>
       </c>
-      <c r="M50" s="57" t="s">
+      <c r="N55" s="196"/>
+      <c r="O55" s="197"/>
+      <c r="P55" s="197"/>
+      <c r="Q55" s="197"/>
+      <c r="R55" s="197"/>
+      <c r="S55" s="196"/>
+      <c r="T55" s="57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="169"/>
-      <c r="E51" s="42" t="s">
+    <row r="56" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="156"/>
+      <c r="E56" s="227"/>
+      <c r="F56" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="103" t="s">
+      <c r="G56" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="L51" s="161"/>
-      <c r="M51" s="57" t="s">
+      <c r="M56" s="163"/>
+      <c r="N56" s="192"/>
+      <c r="T56" s="57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="25" t="s">
+    <row r="57" spans="2:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C57" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="134" t="s">
+      <c r="D57" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="74" t="s">
+      <c r="E57" s="231"/>
+      <c r="F57" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="26" t="s">
+      <c r="G57" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="133" t="s">
+      <c r="H57" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="162" t="s">
-        <v>182</v>
-      </c>
-      <c r="M52" s="60" t="s">
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="173" t="s">
+        <v>179</v>
+      </c>
+      <c r="N57" s="205"/>
+      <c r="O57" s="206"/>
+      <c r="P57" s="206"/>
+      <c r="Q57" s="206"/>
+      <c r="R57" s="206"/>
+      <c r="S57" s="205"/>
+      <c r="T57" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="N52" s="31"/>
-      <c r="O52" s="31"/>
-      <c r="P52" s="31"/>
-      <c r="Q52" s="31"/>
-      <c r="R52" s="31"/>
-      <c r="S52" s="31"/>
-      <c r="T52" s="31"/>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E53" s="42" t="s">
+      <c r="U57" s="31"/>
+      <c r="V57" s="31"/>
+      <c r="W57" s="31"/>
+      <c r="X57" s="31"/>
+      <c r="Y57" s="31"/>
+      <c r="Z57" s="31"/>
+      <c r="AA57" s="31"/>
+    </row>
+    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="E58" s="227"/>
+      <c r="F58" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="G58" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="H58" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L53" s="163"/>
-      <c r="M53" s="57" t="s">
+      <c r="M58" s="174"/>
+      <c r="N58" s="207"/>
+      <c r="O58" s="208"/>
+      <c r="P58" s="208"/>
+      <c r="Q58" s="208"/>
+      <c r="R58" s="208"/>
+      <c r="S58" s="207"/>
+      <c r="T58" s="57" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="164" t="s">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D59" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F59" t="s">
         <v>149</v>
       </c>
-      <c r="F54" s="95" t="s">
+      <c r="G59" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="G54" s="104" t="s">
+      <c r="H59" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="H54" s="105" t="s">
+      <c r="I59" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="151" t="s">
+      <c r="M59" s="162" t="s">
         <v>167</v>
       </c>
-      <c r="M54" s="57" t="s">
+      <c r="N59" s="192"/>
+      <c r="T59" s="57" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="169"/>
-      <c r="E55" t="s">
+    <row r="60" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="156"/>
+      <c r="F60" t="s">
         <v>150</v>
       </c>
-      <c r="F55" s="94" t="s">
+      <c r="G60" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="G55" s="111" t="s">
+      <c r="H60" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="H55" s="115" t="s">
+      <c r="I60" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="161"/>
-      <c r="M55" s="57" t="s">
+      <c r="M60" s="163"/>
+      <c r="N60" s="192"/>
+      <c r="T60" s="57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="25" t="s">
+    <row r="61" spans="2:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C61" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="134" t="s">
+      <c r="D61" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="E56" s="25" t="s">
+      <c r="E61" s="229"/>
+      <c r="F61" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F56" s="26" t="s">
+      <c r="G61" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="H61" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H56" s="27" t="s">
+      <c r="I61" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="150" t="s">
-        <v>182</v>
-      </c>
-      <c r="M56" s="60" t="s">
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="168" t="s">
+        <v>179</v>
+      </c>
+      <c r="N61" s="209"/>
+      <c r="O61" s="210"/>
+      <c r="P61" s="210"/>
+      <c r="Q61" s="210"/>
+      <c r="R61" s="210"/>
+      <c r="S61" s="209"/>
+      <c r="T61" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="N56" s="31"/>
-      <c r="O56" s="31"/>
-      <c r="P56" s="31"/>
-      <c r="Q56" s="31"/>
-      <c r="R56" s="31"/>
-      <c r="S56" s="31"/>
-      <c r="T56" s="31"/>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E57" s="42" t="s">
+      <c r="U61" s="31"/>
+      <c r="V61" s="31"/>
+      <c r="W61" s="31"/>
+      <c r="X61" s="31"/>
+      <c r="Y61" s="31"/>
+      <c r="Z61" s="31"/>
+      <c r="AA61" s="31"/>
+    </row>
+    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="E62" s="227"/>
+      <c r="F62" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="G62" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="98" t="s">
+      <c r="H62" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="151"/>
-      <c r="M57" s="57" t="s">
+      <c r="M62" s="162"/>
+      <c r="N62" s="192"/>
+      <c r="T62" s="57" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="167" t="s">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D63" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="E63" s="227"/>
+      <c r="F63" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F58" s="95" t="s">
+      <c r="G63" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="G58" s="105" t="s">
+      <c r="H63" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="L58" s="151" t="s">
+      <c r="M63" s="162" t="s">
         <v>167</v>
       </c>
-      <c r="M58" s="57" t="s">
+      <c r="N63" s="192"/>
+      <c r="T63" s="57" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="168"/>
-      <c r="E59" s="42" t="s">
+    <row r="64" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="165"/>
+      <c r="E64" s="227"/>
+      <c r="F64" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="F59" s="135" t="s">
+      <c r="G64" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="G59" s="136" t="s">
+      <c r="H64" s="136" t="s">
         <v>64</v>
       </c>
-      <c r="L59" s="161"/>
-      <c r="M59" s="57" t="s">
+      <c r="M64" s="163"/>
+      <c r="N64" s="192"/>
+      <c r="T64" s="57" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F60" s="26"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="60"/>
-      <c r="N60" s="31"/>
-      <c r="O60" s="31"/>
-      <c r="P60" s="31"/>
-      <c r="Q60" s="31"/>
-      <c r="R60" s="31"/>
-      <c r="S60" s="31"/>
-      <c r="T60" s="31"/>
+    <row r="65" spans="5:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="229"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="212"/>
+      <c r="O65" s="212"/>
+      <c r="P65" s="212"/>
+      <c r="Q65" s="212"/>
+      <c r="R65" s="212"/>
+      <c r="S65" s="211"/>
+      <c r="T65" s="60"/>
+      <c r="U65" s="31"/>
+      <c r="V65" s="31"/>
+      <c r="W65" s="31"/>
+      <c r="X65" s="31"/>
+      <c r="Y65" s="31"/>
+      <c r="Z65" s="31"/>
+      <c r="AA65" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="F1:K1"/>
+  <mergeCells count="42">
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="M57:M58"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="M63:M64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A21:A29"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="L58:L59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="L33:L36"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="L56:L57"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="M38:M41"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="M55:M56"/>
+    <mergeCell ref="M59:M60"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3901,23 +4985,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="173" t="s">
+      <c r="F1" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="175"/>
-      <c r="N1" s="173" t="s">
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="178"/>
+      <c r="N1" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="175"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="178"/>
     </row>
     <row r="2" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="160" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -3972,7 +5056,7 @@
       <c r="AA2" s="31"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="153"/>
+      <c r="A3" s="158"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -3996,7 +5080,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="153"/>
+      <c r="A4" s="158"/>
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -4016,7 +5100,7 @@
       <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="153"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -4070,7 +5154,7 @@
       <c r="AA5" s="10"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="153"/>
+      <c r="A6" s="158"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -4094,13 +5178,13 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154"/>
+      <c r="A7" s="159"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="160" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4150,7 +5234,7 @@
       <c r="AA8" s="31"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="154"/>
+      <c r="A9" s="159"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -4177,7 +5261,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="152" t="s">
+      <c r="A10" s="160" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -4221,7 +5305,7 @@
       <c r="AA10" s="31"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="153"/>
+      <c r="A11" s="158"/>
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4239,7 +5323,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="153"/>
+      <c r="A12" s="158"/>
       <c r="D12" t="s">
         <v>3</v>
       </c>
@@ -4251,13 +5335,13 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="153"/>
+      <c r="A13" s="158"/>
       <c r="T13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -4301,7 +5385,7 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="153"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -4328,7 +5412,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="153"/>
+      <c r="A16" s="158"/>
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -4337,7 +5421,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="153"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4381,7 +5465,7 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="153"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
@@ -4408,7 +5492,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="154"/>
+      <c r="A19" s="159"/>
       <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
@@ -4417,7 +5501,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="152" t="s">
+      <c r="A20" s="160" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4459,7 +5543,7 @@
       <c r="AA20" s="31"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="153"/>
+      <c r="A21" s="158"/>
       <c r="D21" t="s">
         <v>4</v>
       </c>
@@ -4474,7 +5558,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="153"/>
+      <c r="A22" s="158"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
@@ -4489,7 +5573,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="153"/>
+      <c r="A23" s="158"/>
       <c r="C23" s="7" t="s">
         <v>44</v>
       </c>
@@ -4526,7 +5610,7 @@
       <c r="AA23" s="10"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="153"/>
+      <c r="A24" s="158"/>
       <c r="D24" t="s">
         <v>45</v>
       </c>
@@ -4541,7 +5625,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="153"/>
+      <c r="A25" s="158"/>
       <c r="D25" t="s">
         <v>46</v>
       </c>
@@ -4556,7 +5640,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="153"/>
+      <c r="A26" s="158"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -4571,7 +5655,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="154"/>
+      <c r="A27" s="159"/>
       <c r="D27" t="s">
         <v>49</v>
       </c>
@@ -4708,14 +5792,14 @@
       <c r="E1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="170" t="s">
+      <c r="F1" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
       <c r="L1" s="116" t="s">
         <v>159</v>
       </c>
@@ -4724,7 +5808,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="160" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -4733,7 +5817,7 @@
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="152" t="s">
+      <c r="D2" s="160" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -4766,8 +5850,8 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="153"/>
-      <c r="D3" s="153"/>
+      <c r="A3" s="158"/>
+      <c r="D3" s="158"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -4780,7 +5864,7 @@
       <c r="H3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="151" t="s">
+      <c r="L3" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="57" t="s">
@@ -4788,8 +5872,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="153"/>
-      <c r="D4" s="172"/>
+      <c r="A4" s="158"/>
+      <c r="D4" s="161"/>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -4800,20 +5884,20 @@
         <v>19</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="L4" s="156"/>
+      <c r="L4" s="167"/>
       <c r="M4" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="153"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="155" t="s">
+      <c r="D5" s="157" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -4846,8 +5930,8 @@
       <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="153"/>
-      <c r="D6" s="153"/>
+      <c r="A6" s="158"/>
+      <c r="D6" s="158"/>
       <c r="E6" t="s">
         <v>2</v>
       </c>
@@ -4860,7 +5944,7 @@
       <c r="H6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="151" t="s">
+      <c r="L6" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="57" t="s">
@@ -4868,18 +5952,18 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154"/>
-      <c r="D7" s="154"/>
+      <c r="A7" s="159"/>
+      <c r="D7" s="159"/>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="156"/>
+      <c r="L7" s="167"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="160" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4888,7 +5972,7 @@
       <c r="C8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="160" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4919,11 +6003,11 @@
       <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="153"/>
+      <c r="A9" s="158"/>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="153"/>
+      <c r="D9" s="158"/>
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -4942,10 +6026,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="153"/>
+      <c r="A10" s="158"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
-      <c r="D10" s="155" t="s">
+      <c r="D10" s="157" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -4974,8 +6058,8 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="154"/>
-      <c r="D11" s="154"/>
+      <c r="A11" s="159"/>
+      <c r="D11" s="159"/>
       <c r="E11" t="s">
         <v>16</v>
       </c>
@@ -4995,7 +6079,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152" t="s">
+      <c r="A12" s="160" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -5033,7 +6117,7 @@
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="153"/>
+      <c r="A13" s="158"/>
       <c r="D13" s="50"/>
       <c r="E13" t="s">
         <v>21</v>
@@ -5053,7 +6137,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
+      <c r="A14" s="158"/>
       <c r="D14" s="52"/>
       <c r="E14" s="53" t="s">
         <v>3</v>
@@ -5077,7 +6161,7 @@
       <c r="T14" s="56"/>
     </row>
     <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="153"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
@@ -5113,7 +6197,7 @@
       <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="153"/>
+      <c r="A16" s="158"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
@@ -5139,7 +6223,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="153"/>
+      <c r="A17" s="158"/>
       <c r="D17" s="50"/>
       <c r="E17" t="s">
         <v>3</v>
@@ -5151,7 +6235,7 @@
       <c r="M17" s="62"/>
     </row>
     <row r="18" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="153"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
@@ -5187,7 +6271,7 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="153"/>
+      <c r="A19" s="158"/>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
@@ -5216,7 +6300,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="154"/>
+      <c r="A20" s="159"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -5230,7 +6314,7 @@
       <c r="L20" s="116"/>
     </row>
     <row r="21" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152" t="s">
+      <c r="A21" s="160" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -5266,7 +6350,7 @@
       <c r="T21" s="31"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="153"/>
+      <c r="A22" s="158"/>
       <c r="D22" s="50"/>
       <c r="E22" t="s">
         <v>45</v>
@@ -5283,7 +6367,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="153"/>
+      <c r="A23" s="158"/>
       <c r="D23" s="50"/>
       <c r="E23" t="s">
         <v>46</v>
@@ -5300,7 +6384,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="153"/>
+      <c r="A24" s="158"/>
       <c r="D24" s="50"/>
       <c r="E24" t="s">
         <v>48</v>
@@ -5317,7 +6401,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="154"/>
+      <c r="A25" s="159"/>
       <c r="D25" s="50"/>
       <c r="E25" t="s">
         <v>49</v>
@@ -5417,7 +6501,7 @@
       <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="164" t="s">
+      <c r="D29" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
@@ -5432,7 +6516,7 @@
       <c r="H29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="151" t="s">
+      <c r="L29" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M29" s="57" t="s">
@@ -5440,7 +6524,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="169"/>
+      <c r="D30" s="156"/>
       <c r="E30" t="s">
         <v>4</v>
       </c>
@@ -5450,10 +6534,10 @@
       <c r="G30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="151"/>
+      <c r="L30" s="162"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="164" t="s">
+      <c r="D31" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
@@ -5468,13 +6552,13 @@
       <c r="H31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="151"/>
+      <c r="L31" s="162"/>
       <c r="M31" s="57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="169"/>
+      <c r="D32" s="156"/>
       <c r="E32" t="s">
         <v>49</v>
       </c>
@@ -5484,7 +6568,7 @@
       <c r="G32" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="L32" s="161"/>
+      <c r="L32" s="163"/>
     </row>
     <row r="33" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
@@ -5542,7 +6626,7 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D35" s="164" t="s">
+      <c r="D35" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -5557,7 +6641,7 @@
       <c r="H35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="151" t="s">
+      <c r="L35" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M35" s="57" t="s">
@@ -5565,7 +6649,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="178"/>
+      <c r="D36" s="179"/>
       <c r="E36" s="43" t="s">
         <v>3</v>
       </c>
@@ -5574,7 +6658,7 @@
       </c>
       <c r="G36" s="46"/>
       <c r="H36" s="65"/>
-      <c r="L36" s="177"/>
+      <c r="L36" s="180"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D37" s="70" t="s">
@@ -5603,7 +6687,7 @@
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D38" s="164" t="s">
+      <c r="D38" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
@@ -5618,7 +6702,7 @@
       <c r="H38" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="151" t="s">
+      <c r="L38" s="162" t="s">
         <v>131</v>
       </c>
       <c r="M38" s="57" t="s">
@@ -5626,7 +6710,7 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D39" s="169"/>
+      <c r="D39" s="156"/>
       <c r="E39" t="s">
         <v>3</v>
       </c>
@@ -5634,10 +6718,10 @@
         <v>29</v>
       </c>
       <c r="H39" s="65"/>
-      <c r="L39" s="151"/>
+      <c r="L39" s="162"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D40" s="164" t="s">
+      <c r="D40" s="155" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -5655,7 +6739,7 @@
       <c r="I40" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="151" t="s">
+      <c r="L40" s="162" t="s">
         <v>103</v>
       </c>
       <c r="M40" s="57" t="s">
@@ -5663,14 +6747,14 @@
       </c>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="169"/>
+      <c r="D41" s="156"/>
       <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="161"/>
+      <c r="L41" s="163"/>
     </row>
     <row r="42" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
@@ -5712,7 +6796,7 @@
       <c r="T42" s="31"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D43" s="164" t="s">
+      <c r="D43" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
@@ -5727,7 +6811,7 @@
       <c r="H43" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="151" t="s">
+      <c r="L43" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M43" s="57" t="s">
@@ -5735,7 +6819,7 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D44" s="169"/>
+      <c r="D44" s="156"/>
       <c r="E44" t="s">
         <v>124</v>
       </c>
@@ -5745,13 +6829,13 @@
       <c r="G44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="151"/>
+      <c r="L44" s="162"/>
       <c r="M44" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D45" s="164" t="s">
+      <c r="D45" s="155" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -5769,7 +6853,7 @@
       <c r="I45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="151" t="s">
+      <c r="L45" s="162" t="s">
         <v>103</v>
       </c>
       <c r="M45" s="57" t="s">
@@ -5777,14 +6861,14 @@
       </c>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="178"/>
+      <c r="D46" s="179"/>
       <c r="E46" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L46" s="177"/>
+      <c r="L46" s="180"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D47" s="70" t="s">
@@ -5833,7 +6917,7 @@
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D49" s="164" t="s">
+      <c r="D49" s="155" t="s">
         <v>73</v>
       </c>
       <c r="E49" t="s">
@@ -5851,7 +6935,7 @@
       <c r="I49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="151" t="s">
+      <c r="L49" s="162" t="s">
         <v>103</v>
       </c>
       <c r="M49" s="57" t="s">
@@ -5859,17 +6943,17 @@
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D50" s="169"/>
+      <c r="D50" s="156"/>
       <c r="E50" t="s">
         <v>91</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="151"/>
+      <c r="L50" s="162"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D51" s="164" t="s">
+      <c r="D51" s="155" t="s">
         <v>74</v>
       </c>
       <c r="E51" t="s">
@@ -5889,14 +6973,14 @@
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="165"/>
+      <c r="D52" s="175"/>
       <c r="E52" t="s">
         <v>127</v>
       </c>
       <c r="F52" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="161"/>
+      <c r="L52" s="163"/>
       <c r="M52" s="57" t="s">
         <v>154</v>
       </c>
@@ -5943,7 +7027,7 @@
       <c r="T53" s="31"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D54" s="164" t="s">
+      <c r="D54" s="155" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="42" t="s">
@@ -5958,7 +7042,7 @@
       <c r="H54" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L54" s="151" t="s">
+      <c r="L54" s="162" t="s">
         <v>102</v>
       </c>
       <c r="M54" s="57" t="s">
@@ -5966,7 +7050,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="176"/>
+      <c r="D55" s="181"/>
       <c r="E55" s="42" t="s">
         <v>4</v>
       </c>
@@ -5977,7 +7061,7 @@
         <v>19</v>
       </c>
       <c r="H55" s="46"/>
-      <c r="L55" s="177"/>
+      <c r="L55" s="180"/>
       <c r="M55" s="57" t="s">
         <v>152</v>
       </c>
@@ -6031,7 +7115,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D58" s="164" t="s">
+      <c r="D58" s="155" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="42" t="s">
@@ -6051,14 +7135,14 @@
       </c>
     </row>
     <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="169"/>
+      <c r="D59" s="156"/>
       <c r="E59" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F59" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="161"/>
+      <c r="L59" s="163"/>
       <c r="M59" s="57" t="s">
         <v>152</v>
       </c>
@@ -6182,7 +7266,7 @@
       </c>
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D65" s="164" t="s">
+      <c r="D65" s="155" t="s">
         <v>74</v>
       </c>
       <c r="E65" t="s">
@@ -6197,7 +7281,7 @@
       <c r="H65" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="L65" s="151" t="s">
+      <c r="L65" s="162" t="s">
         <v>162</v>
       </c>
       <c r="M65" s="57" t="s">
@@ -6205,7 +7289,7 @@
       </c>
     </row>
     <row r="66" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="169"/>
+      <c r="D66" s="156"/>
       <c r="E66" t="s">
         <v>150</v>
       </c>
@@ -6218,7 +7302,7 @@
       <c r="H66" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="L66" s="161"/>
+      <c r="L66" s="163"/>
       <c r="M66" s="57" t="s">
         <v>147</v>
       </c>
@@ -6242,30 +7326,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="L45:L46"/>
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="L58:L59"/>
     <mergeCell ref="D65:D66"/>
@@ -6276,6 +7336,30 @@
     <mergeCell ref="L51:L52"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="L54:L55"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>